<commit_message>
Moved REFPROP2Modelica to Vault
</commit_message>
<xml_diff>
--- a/wrappers/Excel/TestExcel.xlsx
+++ b/wrappers/Excel/TestExcel.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sample calcs" sheetId="1" r:id="rId1"/>
@@ -206,6 +206,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -234,121 +235,121 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>6.1220371700874358E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42.021255884864829</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>83.914144952811213</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>125.7339734191996</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>167.5330355872226</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>209.34176132668546</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>251.18035191395026</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>293.06519282229141</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>335.01235325256681</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>377.03938647775493</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>419.16616289288754</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>461.41518953432177</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>503.81169242146922</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>546.38362438114689</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>589.16169048823406</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>632.17944178056678</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>675.47346558322545</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>719.08369096295633</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>763.05382639583149</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>807.43195145025209</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>852.2712944601858</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>897.63124444416712</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>943.57867004221043</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>990.18965507747396</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1037.5518165790274</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1085.7674588110535</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1134.9579569891293</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1185.2699943566142</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1236.8846659592696</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1290.0311497479677</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1345.0079264161161</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1402.2171260009693</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1462.2236463970921</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1525.8683270564184</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1594.5289922369027</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1670.8899067287159</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1761.6646205625905</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1890.6872488661911</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2060.0042388190018</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -360,121 +361,121 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>0.61165476405738783</c:v>
+                  <c:v>0.61165477790576328</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2281989216218734</c:v>
+                  <c:v>1.2281989260750077</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3393181833843304</c:v>
+                  <c:v>2.3393181837875359</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.2469708453716919</c:v>
+                  <c:v>4.2469708407183706</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.384938078488676</c:v>
+                  <c:v>7.3849380739551265</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.351945839628758</c:v>
+                  <c:v>12.351945840547332</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19.946434302814215</c:v>
+                  <c:v>19.946434302277851</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31.200930025580217</c:v>
+                  <c:v>31.200930025942377</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>47.414474029639273</c:v>
+                  <c:v>47.414474030019207</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>70.181765813260782</c:v>
+                  <c:v>70.181765814537528</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>101.41799666002066</c:v>
+                  <c:v>101.41799666002106</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>143.37871294890778</c:v>
+                  <c:v>143.37871294940228</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>198.67442048006205</c:v>
+                  <c:v>198.67442047934145</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>270.27997678547871</c:v>
+                  <c:v>270.27997678530858</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>361.53909939885102</c:v>
+                  <c:v>361.53909939988046</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>476.16453796963026</c:v>
+                  <c:v>476.16453797031113</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>618.23462142564961</c:v>
+                  <c:v>618.23462142577796</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>792.18700698171995</c:v>
+                  <c:v>792.18700698190401</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1002.8105360783895</c:v>
+                  <c:v>1002.8105360782905</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1255.2361551603883</c:v>
+                  <c:v>1255.2361551605081</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1554.9279004666741</c:v>
+                  <c:v>1554.9279004667762</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1907.6749935323041</c:v>
+                  <c:v>1907.6749935324397</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2319.5861701994427</c:v>
+                  <c:v>2319.5861701998538</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2797.0874969294823</c:v>
+                  <c:v>2797.0874969297211</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3346.9251442691784</c:v>
+                  <c:v>3346.9251442691252</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3976.1749306525894</c:v>
+                  <c:v>3976.1749306524707</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4692.2609922997099</c:v>
+                  <c:v>4692.260992299709</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5502.986783014594</c:v>
+                  <c:v>5502.986783014605</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6416.5829095319705</c:v>
+                  <c:v>6416.582909532026</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7441.7783444211082</c:v>
+                  <c:v>7441.7783444212137</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>8587.9049408354604</c:v>
+                  <c:v>8587.9049408353676</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>9865.0512111821063</c:v>
+                  <c:v>9865.0512111820826</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>11284.292927464845</c:v>
+                  <c:v>11284.292927464725</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>12858.051600018562</c:v>
+                  <c:v>12858.051600018429</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>14600.677371948052</c:v>
+                  <c:v>14600.677371948063</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>16529.415139004024</c:v>
+                  <c:v>16529.415139004064</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>18666.006645644971</c:v>
+                  <c:v>18666.006645644644</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>21043.563147465771</c:v>
+                  <c:v>21043.56314746592</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>22061.3281318503</c:v>
+                  <c:v>22061.328131850038</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -501,121 +502,121 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>2500.9151916490418</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2519.2083189072159</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2537.4334043725835</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2555.545203294766</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2573.510322374003</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2591.2888878672015</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2608.8348722177275</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2626.0964008315318</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2643.0158813452254</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2659.5300141957473</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2675.569884419464</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2691.0613426859572</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2705.9257657931835</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2720.0811051450496</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2733.4429731737559</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2745.9254514300796</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2757.4413489921208</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2767.901762261462</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2777.2149260216215</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2785.28444476205</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2792.0070226267294</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2797.2697683428014</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2800.9470527725625</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2802.8967584010438</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2802.9556046252342</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2800.9330729758303</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2796.6032203853529</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2789.6932193000125</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2779.8667305294548</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2766.6990506391339</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2749.6387614002474</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2727.9458789653859</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2700.5857692409354</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2666.031140557167</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2621.8455755251762</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2563.6367109445468</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2481.4924833322352</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2334.5182916068688</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2110.5585218700166</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -627,121 +628,121 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>0.61165476405738783</c:v>
+                  <c:v>0.61165477790576328</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2281989216218734</c:v>
+                  <c:v>1.2281989260750077</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3393181833843304</c:v>
+                  <c:v>2.3393181837875359</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.2469708453716919</c:v>
+                  <c:v>4.2469708407183706</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.384938078488676</c:v>
+                  <c:v>7.3849380739551265</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.351945839628758</c:v>
+                  <c:v>12.351945840547332</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19.946434302814215</c:v>
+                  <c:v>19.946434302277851</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31.200930025580217</c:v>
+                  <c:v>31.200930025942377</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>47.414474029639273</c:v>
+                  <c:v>47.414474030019207</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>70.181765813260782</c:v>
+                  <c:v>70.181765814537528</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>101.41799666002066</c:v>
+                  <c:v>101.41799666002106</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>143.37871294890778</c:v>
+                  <c:v>143.37871294940228</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>198.67442048006205</c:v>
+                  <c:v>198.67442047934145</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>270.27997678547871</c:v>
+                  <c:v>270.27997678530858</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>361.53909939885102</c:v>
+                  <c:v>361.53909939988046</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>476.16453796963026</c:v>
+                  <c:v>476.16453797031113</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>618.23462142564961</c:v>
+                  <c:v>618.23462142577796</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>792.18700698171995</c:v>
+                  <c:v>792.18700698190401</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1002.8105360783895</c:v>
+                  <c:v>1002.8105360782905</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1255.2361551603883</c:v>
+                  <c:v>1255.2361551605081</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1554.9279004666741</c:v>
+                  <c:v>1554.9279004667762</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1907.6749935323041</c:v>
+                  <c:v>1907.6749935324397</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2319.5861701994427</c:v>
+                  <c:v>2319.5861701998538</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2797.0874969294823</c:v>
+                  <c:v>2797.0874969297211</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3346.9251442691784</c:v>
+                  <c:v>3346.9251442691252</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3976.1749306525894</c:v>
+                  <c:v>3976.1749306524707</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4692.2609922997099</c:v>
+                  <c:v>4692.260992299709</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5502.986783014594</c:v>
+                  <c:v>5502.986783014605</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6416.5829095319705</c:v>
+                  <c:v>6416.582909532026</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7441.7783444211082</c:v>
+                  <c:v>7441.7783444212137</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>8587.9049408354604</c:v>
+                  <c:v>8587.9049408353676</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>9865.0512111821063</c:v>
+                  <c:v>9865.0512111820826</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>11284.292927464845</c:v>
+                  <c:v>11284.292927464725</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>12858.051600018562</c:v>
+                  <c:v>12858.051600018429</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>14600.677371948052</c:v>
+                  <c:v>14600.677371948063</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>16529.415139004024</c:v>
+                  <c:v>16529.415139004064</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>18666.006645644971</c:v>
+                  <c:v>18666.006645644644</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>21043.563147465771</c:v>
+                  <c:v>21043.56314746592</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>22061.3281318503</c:v>
+                  <c:v>22061.328131850038</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -756,11 +757,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="81702272"/>
-        <c:axId val="80142720"/>
+        <c:axId val="119572736"/>
+        <c:axId val="119669120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81702272"/>
+        <c:axId val="119572736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -782,18 +783,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80142720"/>
+        <c:crossAx val="119669120"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80142720"/>
+        <c:axId val="119669120"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -816,13 +818,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81702272"/>
+        <c:crossAx val="119572736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1185,8 +1188,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,7 +1254,7 @@
       </c>
       <c r="B8">
         <f>[1]!Props("T","P",101.325,"Q",0,"Water")-273.15</f>
-        <v>99.974295864387216</v>
+        <v>99.974295847683607</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>10</v>
@@ -1283,8 +1286,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:G44"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1372,23 +1375,23 @@
       </c>
       <c r="C6">
         <f>[1]!Props("P","T",B6,"Q",0,"Water")</f>
-        <v>0.61165476405738783</v>
+        <v>0.61165477790576328</v>
       </c>
       <c r="D6">
         <f>[1]!Props("D","T",B6,"Q",0,"Water")</f>
-        <v>999.79252003840224</v>
+        <v>999.79252003842566</v>
       </c>
       <c r="E6">
         <f>[1]!Props("D","T",B6,"Q",1,"Water")</f>
-        <v>4.8545757582907235E-3</v>
-      </c>
-      <c r="F6">
+        <v>4.8545757582901831E-3</v>
+      </c>
+      <c r="F6" t="e">
         <f>[1]!Props("H","T",B6,"Q",0,"Water")</f>
-        <v>6.1220371700874358E-4</v>
-      </c>
-      <c r="G6">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G6" t="e">
         <f>[1]!Props("H","T",B6,"Q",1,"Water")</f>
-        <v>2500.9151916490418</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1400,24 +1403,24 @@
         <v>283.14999999999998</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:C43" si="1">[1]!Props("P","T",B7,"Q",0,"Water")</f>
-        <v>1.2281989216218734</v>
+        <f>[1]!Props("P","T",B7,"Q",0,"Water")</f>
+        <v>1.2281989260750077</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:D43" si="2">[1]!Props("D","T",B7,"Q",0,"Water")</f>
-        <v>999.65462464160316</v>
+        <f>[1]!Props("D","T",B7,"Q",0,"Water")</f>
+        <v>999.65462464159361</v>
       </c>
       <c r="E7">
-        <f t="shared" ref="E7:E43" si="3">[1]!Props("D","T",B7,"Q",1,"Water")</f>
-        <v>9.4070520080235566E-3</v>
-      </c>
-      <c r="F7">
-        <f t="shared" ref="F7:F43" si="4">[1]!Props("H","T",B7,"Q",0,"Water")</f>
-        <v>42.021255884864829</v>
-      </c>
-      <c r="G7">
-        <f t="shared" ref="G7:G43" si="5">[1]!Props("H","T",B7,"Q",1,"Water")</f>
-        <v>2519.2083189072159</v>
+        <f>[1]!Props("D","T",B7,"Q",1,"Water")</f>
+        <v>9.4070520080230726E-3</v>
+      </c>
+      <c r="F7" t="e">
+        <f>[1]!Props("H","T",B7,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G7" t="e">
+        <f>[1]!Props("H","T",B7,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1429,24 +1432,24 @@
         <v>293.14999999999998</v>
       </c>
       <c r="C8">
-        <f t="shared" si="1"/>
-        <v>2.3393181833843304</v>
+        <f>[1]!Props("P","T",B8,"Q",0,"Water")</f>
+        <v>2.3393181837875359</v>
       </c>
       <c r="D8">
-        <f t="shared" si="2"/>
-        <v>998.16180134316789</v>
+        <f>[1]!Props("D","T",B8,"Q",0,"Water")</f>
+        <v>998.16180134317437</v>
       </c>
       <c r="E8">
-        <f t="shared" si="3"/>
-        <v>1.7314008205457702E-2</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="4"/>
-        <v>83.914144952811213</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="5"/>
-        <v>2537.4334043725835</v>
+        <f>[1]!Props("D","T",B8,"Q",1,"Water")</f>
+        <v>1.7314008205457157E-2</v>
+      </c>
+      <c r="F8" t="e">
+        <f>[1]!Props("H","T",B8,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G8" t="e">
+        <f>[1]!Props("H","T",B8,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1458,24 +1461,24 @@
         <v>303.14999999999998</v>
       </c>
       <c r="C9">
-        <f t="shared" si="1"/>
-        <v>4.2469708453716919</v>
+        <f>[1]!Props("P","T",B9,"Q",0,"Water")</f>
+        <v>4.2469708407183706</v>
       </c>
       <c r="D9">
-        <f t="shared" si="2"/>
-        <v>995.60617747384254</v>
+        <f>[1]!Props("D","T",B9,"Q",0,"Water")</f>
+        <v>995.60617747384663</v>
       </c>
       <c r="E9">
-        <f t="shared" si="3"/>
-        <v>3.0415211808982469E-2</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="4"/>
-        <v>125.7339734191996</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="5"/>
-        <v>2555.545203294766</v>
+        <f>[1]!Props("D","T",B9,"Q",1,"Water")</f>
+        <v>3.0415211808982323E-2</v>
+      </c>
+      <c r="F9" t="e">
+        <f>[1]!Props("H","T",B9,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G9" t="e">
+        <f>[1]!Props("H","T",B9,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1487,24 +1490,24 @@
         <v>313.14999999999998</v>
       </c>
       <c r="C10">
-        <f t="shared" si="1"/>
-        <v>7.384938078488676</v>
+        <f>[1]!Props("P","T",B10,"Q",0,"Water")</f>
+        <v>7.3849380739551265</v>
       </c>
       <c r="D10">
-        <f t="shared" si="2"/>
-        <v>992.17511534129972</v>
+        <f>[1]!Props("D","T",B10,"Q",0,"Water")</f>
+        <v>992.17511534129721</v>
       </c>
       <c r="E10">
-        <f t="shared" si="3"/>
-        <v>5.1242255801689604E-2</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="4"/>
-        <v>167.5330355872226</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="5"/>
-        <v>2573.510322374003</v>
+        <f>[1]!Props("D","T",B10,"Q",1,"Water")</f>
+        <v>5.1242255801689097E-2</v>
+      </c>
+      <c r="F10" t="e">
+        <f>[1]!Props("H","T",B10,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G10" t="e">
+        <f>[1]!Props("H","T",B10,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1516,24 +1519,24 @@
         <v>323.14999999999998</v>
       </c>
       <c r="C11">
-        <f t="shared" si="1"/>
-        <v>12.351945839628758</v>
+        <f>[1]!Props("P","T",B11,"Q",0,"Water")</f>
+        <v>12.351945840547332</v>
       </c>
       <c r="D11">
-        <f t="shared" si="2"/>
-        <v>987.99621061117341</v>
+        <f>[1]!Props("D","T",B11,"Q",0,"Water")</f>
+        <v>987.9962106111717</v>
       </c>
       <c r="E11">
-        <f t="shared" si="3"/>
-        <v>8.3146842800444973E-2</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="4"/>
-        <v>209.34176132668546</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="5"/>
-        <v>2591.2888878672015</v>
+        <f>[1]!Props("D","T",B11,"Q",1,"Water")</f>
+        <v>8.3146842800445916E-2</v>
+      </c>
+      <c r="F11" t="e">
+        <f>[1]!Props("H","T",B11,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G11" t="e">
+        <f>[1]!Props("H","T",B11,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1545,24 +1548,24 @@
         <v>333.15</v>
       </c>
       <c r="C12">
-        <f t="shared" si="1"/>
-        <v>19.946434302814215</v>
+        <f>[1]!Props("P","T",B12,"Q",0,"Water")</f>
+        <v>19.946434302277851</v>
       </c>
       <c r="D12">
-        <f t="shared" si="2"/>
-        <v>983.16021717833291</v>
+        <f>[1]!Props("D","T",B12,"Q",0,"Water")</f>
+        <v>983.16021717833303</v>
       </c>
       <c r="E12">
-        <f t="shared" si="3"/>
-        <v>0.13042522259659811</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="4"/>
-        <v>251.18035191395026</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="5"/>
-        <v>2608.8348722177275</v>
+        <f>[1]!Props("D","T",B12,"Q",1,"Water")</f>
+        <v>0.13042522259659625</v>
+      </c>
+      <c r="F12" t="e">
+        <f>[1]!Props("H","T",B12,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G12" t="e">
+        <f>[1]!Props("H","T",B12,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1574,24 +1577,24 @@
         <v>343.15</v>
       </c>
       <c r="C13">
-        <f t="shared" si="1"/>
-        <v>31.200930025580217</v>
+        <f>[1]!Props("P","T",B13,"Q",0,"Water")</f>
+        <v>31.200930025942377</v>
       </c>
       <c r="D13">
-        <f t="shared" si="2"/>
-        <v>977.73365598192902</v>
+        <f>[1]!Props("D","T",B13,"Q",0,"Water")</f>
+        <v>977.73365598192868</v>
       </c>
       <c r="E13">
-        <f t="shared" si="3"/>
-        <v>0.19843073794182256</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="4"/>
-        <v>293.06519282229141</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="5"/>
-        <v>2626.0964008315318</v>
+        <f>[1]!Props("D","T",B13,"Q",1,"Water")</f>
+        <v>0.19843073794182545</v>
+      </c>
+      <c r="F13" t="e">
+        <f>[1]!Props("H","T",B13,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G13" t="e">
+        <f>[1]!Props("H","T",B13,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1603,24 +1606,24 @@
         <v>353.15</v>
       </c>
       <c r="C14">
-        <f t="shared" si="1"/>
-        <v>47.414474029639273</v>
+        <f>[1]!Props("P","T",B14,"Q",0,"Water")</f>
+        <v>47.414474030019207</v>
       </c>
       <c r="D14">
-        <f t="shared" si="2"/>
-        <v>971.76621871051191</v>
+        <f>[1]!Props("D","T",B14,"Q",0,"Water")</f>
+        <v>971.76621871051145</v>
       </c>
       <c r="E14">
-        <f t="shared" si="3"/>
-        <v>0.29367213474273518</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="4"/>
-        <v>335.01235325256681</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="5"/>
-        <v>2643.0158813452254</v>
+        <f>[1]!Props("D","T",B14,"Q",1,"Water")</f>
+        <v>0.2936721347427359</v>
+      </c>
+      <c r="F14" t="e">
+        <f>[1]!Props("H","T",B14,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G14" t="e">
+        <f>[1]!Props("H","T",B14,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1632,24 +1635,24 @@
         <v>363.15</v>
       </c>
       <c r="C15">
-        <f t="shared" si="1"/>
-        <v>70.181765813260782</v>
+        <f>[1]!Props("P","T",B15,"Q",0,"Water")</f>
+        <v>70.181765814537528</v>
       </c>
       <c r="D15">
-        <f t="shared" si="2"/>
-        <v>965.29532855043726</v>
+        <f>[1]!Props("D","T",B15,"Q",0,"Water")</f>
+        <v>965.29532855043715</v>
       </c>
       <c r="E15">
-        <f t="shared" si="3"/>
-        <v>0.42389794463172359</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="4"/>
-        <v>377.03938647775493</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="5"/>
-        <v>2659.5300141957473</v>
+        <f>[1]!Props("D","T",B15,"Q",1,"Water")</f>
+        <v>0.42389794463171637</v>
+      </c>
+      <c r="F15" t="e">
+        <f>[1]!Props("H","T",B15,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G15" t="e">
+        <f>[1]!Props("H","T",B15,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1661,24 +1664,24 @@
         <v>373.15</v>
       </c>
       <c r="C16">
-        <f t="shared" si="1"/>
-        <v>101.41799666002066</v>
+        <f>[1]!Props("P","T",B16,"Q",0,"Water")</f>
+        <v>101.41799666002106</v>
       </c>
       <c r="D16">
-        <f t="shared" si="2"/>
+        <f>[1]!Props("D","T",B16,"Q",0,"Water")</f>
         <v>958.34905160486005</v>
       </c>
       <c r="E16">
-        <f t="shared" si="3"/>
-        <v>0.59816979192597053</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="4"/>
-        <v>419.16616289288754</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="5"/>
-        <v>2675.569884419464</v>
+        <f>[1]!Props("D","T",B16,"Q",1,"Water")</f>
+        <v>0.5981697919259753</v>
+      </c>
+      <c r="F16" t="e">
+        <f>[1]!Props("H","T",B16,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G16" t="e">
+        <f>[1]!Props("H","T",B16,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1690,24 +1693,24 @@
         <v>383.15</v>
       </c>
       <c r="C17">
-        <f t="shared" si="1"/>
-        <v>143.37871294890778</v>
+        <f>[1]!Props("P","T",B17,"Q",0,"Water")</f>
+        <v>143.37871294940228</v>
       </c>
       <c r="D17">
-        <f t="shared" si="2"/>
-        <v>950.94800358896453</v>
+        <f>[1]!Props("D","T",B17,"Q",0,"Water")</f>
+        <v>950.9480035889643</v>
       </c>
       <c r="E17">
-        <f t="shared" si="3"/>
-        <v>0.8269295957235937</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="4"/>
-        <v>461.41518953432177</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="5"/>
-        <v>2691.0613426859572</v>
+        <f>[1]!Props("D","T",B17,"Q",1,"Water")</f>
+        <v>0.82692959572358737</v>
+      </c>
+      <c r="F17" t="e">
+        <f>[1]!Props("H","T",B17,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G17" t="e">
+        <f>[1]!Props("H","T",B17,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1719,24 +1722,24 @@
         <v>393.15</v>
       </c>
       <c r="C18">
-        <f t="shared" si="1"/>
-        <v>198.67442048006205</v>
+        <f>[1]!Props("P","T",B18,"Q",0,"Water")</f>
+        <v>198.67442047934145</v>
       </c>
       <c r="D18">
-        <f t="shared" si="2"/>
-        <v>943.10661743025378</v>
+        <f>[1]!Props("D","T",B18,"Q",0,"Water")</f>
+        <v>943.106617430254</v>
       </c>
       <c r="E18">
-        <f t="shared" si="3"/>
-        <v>1.1220671917645149</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="4"/>
-        <v>503.81169242146922</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="5"/>
-        <v>2705.9257657931835</v>
+        <f>[1]!Props("D","T",B18,"Q",1,"Water")</f>
+        <v>1.1220671917645244</v>
+      </c>
+      <c r="F18" t="e">
+        <f>[1]!Props("H","T",B18,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G18" t="e">
+        <f>[1]!Props("H","T",B18,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1748,24 +1751,24 @@
         <v>403.15</v>
       </c>
       <c r="C19">
-        <f t="shared" si="1"/>
-        <v>270.27997678547871</v>
+        <f>[1]!Props("P","T",B19,"Q",0,"Water")</f>
+        <v>270.27997678530858</v>
       </c>
       <c r="D19">
-        <f t="shared" si="2"/>
-        <v>934.83398660707996</v>
+        <f>[1]!Props("D","T",B19,"Q",0,"Water")</f>
+        <v>934.83398660707985</v>
       </c>
       <c r="E19">
-        <f t="shared" si="3"/>
-        <v>1.4969959714829018</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="4"/>
-        <v>546.38362438114689</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="5"/>
-        <v>2720.0811051450496</v>
+        <f>[1]!Props("D","T",B19,"Q",1,"Water")</f>
+        <v>1.4969959714828884</v>
+      </c>
+      <c r="F19" t="e">
+        <f>[1]!Props("H","T",B19,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G19" t="e">
+        <f>[1]!Props("H","T",B19,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1777,24 +1780,24 @@
         <v>413.15</v>
       </c>
       <c r="C20">
-        <f t="shared" si="1"/>
-        <v>361.53909939885102</v>
+        <f>[1]!Props("P","T",B20,"Q",0,"Water")</f>
+        <v>361.53909939988046</v>
       </c>
       <c r="D20">
-        <f t="shared" si="2"/>
-        <v>926.13441329112425</v>
+        <f>[1]!Props("D","T",B20,"Q",0,"Water")</f>
+        <v>926.13441329112413</v>
       </c>
       <c r="E20">
-        <f t="shared" si="3"/>
-        <v>1.9667450045125203</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="4"/>
-        <v>589.16169048823406</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="5"/>
-        <v>2733.4429731737559</v>
+        <f>[1]!Props("D","T",B20,"Q",1,"Water")</f>
+        <v>1.9667450045125305</v>
+      </c>
+      <c r="F20" t="e">
+        <f>[1]!Props("H","T",B20,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G20" t="e">
+        <f>[1]!Props("H","T",B20,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1806,24 +1809,24 @@
         <v>423.15</v>
       </c>
       <c r="C21">
-        <f t="shared" si="1"/>
-        <v>476.16453796963026</v>
+        <f>[1]!Props("P","T",B21,"Q",0,"Water")</f>
+        <v>476.16453797031113</v>
       </c>
       <c r="D21">
-        <f t="shared" si="2"/>
-        <v>917.00773926892509</v>
+        <f>[1]!Props("D","T",B21,"Q",0,"Water")</f>
+        <v>917.00773926892555</v>
       </c>
       <c r="E21">
-        <f t="shared" si="3"/>
-        <v>2.5480771470961106</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="4"/>
-        <v>632.17944178056678</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="5"/>
-        <v>2745.9254514300796</v>
+        <f>[1]!Props("D","T",B21,"Q",1,"Water")</f>
+        <v>2.5480771470961141</v>
+      </c>
+      <c r="F21" t="e">
+        <f>[1]!Props("H","T",B21,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G21" t="e">
+        <f>[1]!Props("H","T",B21,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1835,24 +1838,24 @@
         <v>433.15</v>
       </c>
       <c r="C22">
-        <f t="shared" si="1"/>
-        <v>618.23462142564961</v>
+        <f>[1]!Props("P","T",B22,"Q",0,"Water")</f>
+        <v>618.23462142577796</v>
       </c>
       <c r="D22">
-        <f t="shared" si="2"/>
-        <v>907.4495056340736</v>
+        <f>[1]!Props("D","T",B22,"Q",0,"Water")</f>
+        <v>907.44950563407349</v>
       </c>
       <c r="E22">
-        <f t="shared" si="3"/>
-        <v>3.2596441977608315</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="4"/>
-        <v>675.47346558322545</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="5"/>
-        <v>2757.4413489921208</v>
+        <f>[1]!Props("D","T",B22,"Q",1,"Water")</f>
+        <v>3.2596441977608386</v>
+      </c>
+      <c r="F22" t="e">
+        <f>[1]!Props("H","T",B22,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G22" t="e">
+        <f>[1]!Props("H","T",B22,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1864,24 +1867,24 @@
         <v>443.15</v>
       </c>
       <c r="C23">
-        <f t="shared" si="1"/>
-        <v>792.18700698171995</v>
+        <f>[1]!Props("P","T",B23,"Q",0,"Water")</f>
+        <v>792.18700698190401</v>
       </c>
       <c r="D23">
-        <f t="shared" si="2"/>
-        <v>897.45096587597243</v>
+        <f>[1]!Props("D","T",B23,"Q",0,"Water")</f>
+        <v>897.45096587597288</v>
       </c>
       <c r="E23">
-        <f t="shared" si="3"/>
-        <v>4.1221925343361461</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="4"/>
-        <v>719.08369096295633</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="5"/>
-        <v>2767.901762261462</v>
+        <f>[1]!Props("D","T",B23,"Q",1,"Water")</f>
+        <v>4.1221925343361514</v>
+      </c>
+      <c r="F23" t="e">
+        <f>[1]!Props("H","T",B23,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G23" t="e">
+        <f>[1]!Props("H","T",B23,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1893,24 +1896,24 @@
         <v>453.15</v>
       </c>
       <c r="C24">
-        <f t="shared" si="1"/>
-        <v>1002.8105360783895</v>
+        <f>[1]!Props("P","T",B24,"Q",0,"Water")</f>
+        <v>1002.8105360782905</v>
       </c>
       <c r="D24">
-        <f t="shared" si="2"/>
+        <f>[1]!Props("D","T",B24,"Q",0,"Water")</f>
         <v>886.99896128082025</v>
       </c>
       <c r="E24">
-        <f t="shared" si="3"/>
-        <v>5.1588361289185167</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="4"/>
-        <v>763.05382639583149</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="5"/>
-        <v>2777.2149260216215</v>
+        <f>[1]!Props("D","T",B24,"Q",1,"Water")</f>
+        <v>5.1588361289185185</v>
+      </c>
+      <c r="F24" t="e">
+        <f>[1]!Props("H","T",B24,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G24" t="e">
+        <f>[1]!Props("H","T",B24,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1922,24 +1925,24 @@
         <v>463.15</v>
       </c>
       <c r="C25">
-        <f t="shared" si="1"/>
-        <v>1255.2361551603883</v>
+        <f>[1]!Props("P","T",B25,"Q",0,"Water")</f>
+        <v>1255.2361551605081</v>
       </c>
       <c r="D25">
-        <f t="shared" si="2"/>
-        <v>876.07565429885631</v>
+        <f>[1]!Props("D","T",B25,"Q",0,"Water")</f>
+        <v>876.07565429885642</v>
       </c>
       <c r="E25">
-        <f t="shared" si="3"/>
-        <v>6.3954187812078507</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="4"/>
-        <v>807.43195145025209</v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="5"/>
-        <v>2785.28444476205</v>
+        <f>[1]!Props("D","T",B25,"Q",1,"Water")</f>
+        <v>6.3954187812079395</v>
+      </c>
+      <c r="F25" t="e">
+        <f>[1]!Props("H","T",B25,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G25" t="e">
+        <f>[1]!Props("H","T",B25,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1951,24 +1954,24 @@
         <v>473.15</v>
       </c>
       <c r="C26">
-        <f t="shared" si="1"/>
-        <v>1554.9279004666741</v>
+        <f>[1]!Props("P","T",B26,"Q",0,"Water")</f>
+        <v>1554.9279004667762</v>
       </c>
       <c r="D26">
-        <f t="shared" si="2"/>
-        <v>864.65810228712587</v>
+        <f>[1]!Props("D","T",B26,"Q",0,"Water")</f>
+        <v>864.65810228712542</v>
       </c>
       <c r="E26">
-        <f t="shared" si="3"/>
-        <v>7.8609945167840447</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="4"/>
-        <v>852.2712944601858</v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="5"/>
-        <v>2792.0070226267294</v>
+        <f>[1]!Props("D","T",B26,"Q",1,"Water")</f>
+        <v>7.860994516784042</v>
+      </c>
+      <c r="F26" t="e">
+        <f>[1]!Props("H","T",B26,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G26" t="e">
+        <f>[1]!Props("H","T",B26,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1980,24 +1983,24 @@
         <v>483.15</v>
       </c>
       <c r="C27">
-        <f t="shared" si="1"/>
-        <v>1907.6749935323041</v>
+        <f>[1]!Props("P","T",B27,"Q",0,"Water")</f>
+        <v>1907.6749935324397</v>
       </c>
       <c r="D27">
-        <f t="shared" si="2"/>
-        <v>852.71763851005699</v>
+        <f>[1]!Props("D","T",B27,"Q",0,"Water")</f>
+        <v>852.71763851005721</v>
       </c>
       <c r="E27">
-        <f t="shared" si="3"/>
-        <v>9.5884655414267801</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="4"/>
-        <v>897.63124444416712</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="5"/>
-        <v>2797.2697683428014</v>
+        <f>[1]!Props("D","T",B27,"Q",1,"Water")</f>
+        <v>9.5884655414267677</v>
+      </c>
+      <c r="F27" t="e">
+        <f>[1]!Props("H","T",B27,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G27" t="e">
+        <f>[1]!Props("H","T",B27,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -2009,24 +2012,24 @@
         <v>493.15</v>
       </c>
       <c r="C28">
-        <f t="shared" si="1"/>
-        <v>2319.5861701994427</v>
+        <f>[1]!Props("P","T",B28,"Q",0,"Water")</f>
+        <v>2319.5861701998538</v>
       </c>
       <c r="D28">
-        <f t="shared" si="2"/>
-        <v>840.21900675000279</v>
+        <f>[1]!Props("D","T",B28,"Q",0,"Water")</f>
+        <v>840.21900675000336</v>
       </c>
       <c r="E28">
-        <f t="shared" si="3"/>
-        <v>11.615432874295013</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="4"/>
-        <v>943.57867004221043</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="5"/>
-        <v>2800.9470527725625</v>
+        <f>[1]!Props("D","T",B28,"Q",1,"Water")</f>
+        <v>11.615432874295058</v>
+      </c>
+      <c r="F28" t="e">
+        <f>[1]!Props("H","T",B28,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G28" t="e">
+        <f>[1]!Props("H","T",B28,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -2038,24 +2041,24 @@
         <v>503.15</v>
       </c>
       <c r="C29">
-        <f t="shared" si="1"/>
-        <v>2797.0874969294823</v>
+        <f>[1]!Props("P","T",B29,"Q",0,"Water")</f>
+        <v>2797.0874969297211</v>
       </c>
       <c r="D29">
-        <f t="shared" si="2"/>
-        <v>827.11916655179903</v>
+        <f>[1]!Props("D","T",B29,"Q",0,"Water")</f>
+        <v>827.11916655179948</v>
       </c>
       <c r="E29">
-        <f t="shared" si="3"/>
-        <v>13.985338957508485</v>
-      </c>
-      <c r="F29">
-        <f t="shared" si="4"/>
-        <v>990.18965507747396</v>
-      </c>
-      <c r="G29">
-        <f t="shared" si="5"/>
-        <v>2802.8967584010438</v>
+        <f>[1]!Props("D","T",B29,"Q",1,"Water")</f>
+        <v>13.98533895750848</v>
+      </c>
+      <c r="F29" t="e">
+        <f>[1]!Props("H","T",B29,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G29" t="e">
+        <f>[1]!Props("H","T",B29,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -2067,24 +2070,24 @@
         <v>513.15</v>
       </c>
       <c r="C30">
-        <f t="shared" si="1"/>
-        <v>3346.9251442691784</v>
+        <f>[1]!Props("P","T",B30,"Q",0,"Water")</f>
+        <v>3346.9251442691252</v>
       </c>
       <c r="D30">
-        <f t="shared" si="2"/>
+        <f>[1]!Props("D","T",B30,"Q",0,"Water")</f>
         <v>813.36564216909892</v>
       </c>
       <c r="E30">
-        <f t="shared" si="3"/>
-        <v>16.749019301603237</v>
-      </c>
-      <c r="F30">
-        <f t="shared" si="4"/>
-        <v>1037.5518165790274</v>
-      </c>
-      <c r="G30">
-        <f t="shared" si="5"/>
-        <v>2802.9556046252342</v>
+        <f>[1]!Props("D","T",B30,"Q",1,"Water")</f>
+        <v>16.749019301603251</v>
+      </c>
+      <c r="F30" t="e">
+        <f>[1]!Props("H","T",B30,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G30" t="e">
+        <f>[1]!Props("H","T",B30,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -2096,24 +2099,24 @@
         <v>523.15</v>
       </c>
       <c r="C31">
-        <f t="shared" si="1"/>
-        <v>3976.1749306525894</v>
+        <f>[1]!Props("P","T",B31,"Q",0,"Water")</f>
+        <v>3976.1749306524707</v>
       </c>
       <c r="D31">
-        <f t="shared" si="2"/>
-        <v>798.89422022042197</v>
+        <f>[1]!Props("D","T",B31,"Q",0,"Water")</f>
+        <v>798.89422022042186</v>
       </c>
       <c r="E31">
-        <f t="shared" si="3"/>
-        <v>19.966840438464846</v>
-      </c>
-      <c r="F31">
-        <f t="shared" si="4"/>
-        <v>1085.7674588110535</v>
-      </c>
-      <c r="G31">
-        <f t="shared" si="5"/>
-        <v>2800.9330729758303</v>
+        <f>[1]!Props("D","T",B31,"Q",1,"Water")</f>
+        <v>19.966840438464651</v>
+      </c>
+      <c r="F31" t="e">
+        <f>[1]!Props("H","T",B31,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G31" t="e">
+        <f>[1]!Props("H","T",B31,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -2125,24 +2128,24 @@
         <v>533.15</v>
       </c>
       <c r="C32">
-        <f t="shared" si="1"/>
-        <v>4692.2609922997099</v>
+        <f>[1]!Props("P","T",B32,"Q",0,"Water")</f>
+        <v>4692.260992299709</v>
       </c>
       <c r="D32">
-        <f t="shared" si="2"/>
+        <f>[1]!Props("D","T",B32,"Q",0,"Water")</f>
         <v>783.62569286973383</v>
       </c>
       <c r="E32">
-        <f t="shared" si="3"/>
-        <v>23.711700367712282</v>
-      </c>
-      <c r="F32">
-        <f t="shared" si="4"/>
-        <v>1134.9579569891293</v>
-      </c>
-      <c r="G32">
-        <f t="shared" si="5"/>
-        <v>2796.6032203853529</v>
+        <f>[1]!Props("D","T",B32,"Q",1,"Water")</f>
+        <v>23.711700367712265</v>
+      </c>
+      <c r="F32" t="e">
+        <f>[1]!Props("H","T",B32,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G32" t="e">
+        <f>[1]!Props("H","T",B32,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -2154,24 +2157,24 @@
         <v>543.15</v>
       </c>
       <c r="C33">
-        <f t="shared" si="1"/>
-        <v>5502.986783014594</v>
+        <f>[1]!Props("P","T",B33,"Q",0,"Water")</f>
+        <v>5502.986783014605</v>
       </c>
       <c r="D33">
-        <f t="shared" si="2"/>
-        <v>767.46116679898091</v>
+        <f>[1]!Props("D","T",B33,"Q",0,"Water")</f>
+        <v>767.46116679898125</v>
       </c>
       <c r="E33">
-        <f t="shared" si="3"/>
-        <v>28.073335624424175</v>
-      </c>
-      <c r="F33">
-        <f t="shared" si="4"/>
-        <v>1185.2699943566142</v>
-      </c>
-      <c r="G33">
-        <f t="shared" si="5"/>
-        <v>2789.6932193000125</v>
+        <f>[1]!Props("D","T",B33,"Q",1,"Water")</f>
+        <v>28.07333562442464</v>
+      </c>
+      <c r="F33" t="e">
+        <f>[1]!Props("H","T",B33,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G33" t="e">
+        <f>[1]!Props("H","T",B33,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -2183,24 +2186,24 @@
         <v>553.15</v>
       </c>
       <c r="C34">
-        <f t="shared" si="1"/>
-        <v>6416.5829095319705</v>
+        <f>[1]!Props("P","T",B34,"Q",0,"Water")</f>
+        <v>6416.582909532026</v>
       </c>
       <c r="D34">
-        <f t="shared" si="2"/>
-        <v>750.27516129988305</v>
+        <f>[1]!Props("D","T",B34,"Q",0,"Water")</f>
+        <v>750.27516129988351</v>
       </c>
       <c r="E34">
-        <f t="shared" si="3"/>
-        <v>33.164674054045747</v>
-      </c>
-      <c r="F34">
-        <f t="shared" si="4"/>
-        <v>1236.8846659592696</v>
-      </c>
-      <c r="G34">
-        <f t="shared" si="5"/>
-        <v>2779.8667305294548</v>
+        <f>[1]!Props("D","T",B34,"Q",1,"Water")</f>
+        <v>33.164674054045683</v>
+      </c>
+      <c r="F34" t="e">
+        <f>[1]!Props("H","T",B34,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G34" t="e">
+        <f>[1]!Props("H","T",B34,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -2212,24 +2215,24 @@
         <v>563.15</v>
       </c>
       <c r="C35">
-        <f t="shared" si="1"/>
-        <v>7441.7783444211082</v>
+        <f>[1]!Props("P","T",B35,"Q",0,"Water")</f>
+        <v>7441.7783444212137</v>
       </c>
       <c r="D35">
-        <f t="shared" si="2"/>
-        <v>731.90519964368616</v>
+        <f>[1]!Props("D","T",B35,"Q",0,"Water")</f>
+        <v>731.9051996436865</v>
       </c>
       <c r="E35">
-        <f t="shared" si="3"/>
-        <v>39.131512960158574</v>
-      </c>
-      <c r="F35">
-        <f t="shared" si="4"/>
-        <v>1290.0311497479677</v>
-      </c>
-      <c r="G35">
-        <f t="shared" si="5"/>
-        <v>2766.6990506391339</v>
+        <f>[1]!Props("D","T",B35,"Q",1,"Water")</f>
+        <v>39.131512960158695</v>
+      </c>
+      <c r="F35" t="e">
+        <f>[1]!Props("H","T",B35,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G35" t="e">
+        <f>[1]!Props("H","T",B35,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -2241,24 +2244,24 @@
         <v>573.15</v>
       </c>
       <c r="C36">
-        <f t="shared" si="1"/>
-        <v>8587.9049408354604</v>
+        <f>[1]!Props("P","T",B36,"Q",0,"Water")</f>
+        <v>8587.9049408353676</v>
       </c>
       <c r="D36">
-        <f t="shared" si="2"/>
-        <v>712.1356388196142</v>
+        <f>[1]!Props("D","T",B36,"Q",0,"Water")</f>
+        <v>712.13563881961431</v>
       </c>
       <c r="E36">
-        <f t="shared" si="3"/>
-        <v>46.167849523794544</v>
-      </c>
-      <c r="F36">
-        <f t="shared" si="4"/>
-        <v>1345.0079264161161</v>
-      </c>
-      <c r="G36">
-        <f t="shared" si="5"/>
-        <v>2749.6387614002474</v>
+        <f>[1]!Props("D","T",B36,"Q",1,"Water")</f>
+        <v>46.167849523794111</v>
+      </c>
+      <c r="F36" t="e">
+        <f>[1]!Props("H","T",B36,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G36" t="e">
+        <f>[1]!Props("H","T",B36,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -2270,24 +2273,24 @@
         <v>583.15</v>
       </c>
       <c r="C37">
-        <f t="shared" si="1"/>
-        <v>9865.0512111821063</v>
+        <f>[1]!Props("P","T",B37,"Q",0,"Water")</f>
+        <v>9865.0512111820826</v>
       </c>
       <c r="D37">
-        <f t="shared" si="2"/>
-        <v>690.67154560984386</v>
+        <f>[1]!Props("D","T",B37,"Q",0,"Water")</f>
+        <v>690.67154560984363</v>
       </c>
       <c r="E37">
-        <f t="shared" si="3"/>
-        <v>54.541361541638295</v>
-      </c>
-      <c r="F37">
-        <f t="shared" si="4"/>
-        <v>1402.2171260009693</v>
-      </c>
-      <c r="G37">
-        <f t="shared" si="5"/>
-        <v>2727.9458789653859</v>
+        <f>[1]!Props("D","T",B37,"Q",1,"Water")</f>
+        <v>54.541361541638153</v>
+      </c>
+      <c r="F37" t="e">
+        <f>[1]!Props("H","T",B37,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G37" t="e">
+        <f>[1]!Props("H","T",B37,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -2299,24 +2302,24 @@
         <v>593.15</v>
       </c>
       <c r="C38">
-        <f t="shared" si="1"/>
-        <v>11284.292927464845</v>
+        <f>[1]!Props("P","T",B38,"Q",0,"Water")</f>
+        <v>11284.292927464725</v>
       </c>
       <c r="D38">
-        <f t="shared" si="2"/>
-        <v>667.09384803259536</v>
+        <f>[1]!Props("D","T",B38,"Q",0,"Water")</f>
+        <v>667.09384803259525</v>
       </c>
       <c r="E38">
-        <f t="shared" si="3"/>
-        <v>64.638432419886243</v>
-      </c>
-      <c r="F38">
-        <f t="shared" si="4"/>
-        <v>1462.2236463970921</v>
-      </c>
-      <c r="G38">
-        <f t="shared" si="5"/>
-        <v>2700.5857692409354</v>
+        <f>[1]!Props("D","T",B38,"Q",1,"Water")</f>
+        <v>64.638432419886186</v>
+      </c>
+      <c r="F38" t="e">
+        <f>[1]!Props("H","T",B38,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G38" t="e">
+        <f>[1]!Props("H","T",B38,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -2328,24 +2331,24 @@
         <v>603.15</v>
       </c>
       <c r="C39">
-        <f t="shared" si="1"/>
-        <v>12858.051600018562</v>
+        <f>[1]!Props("P","T",B39,"Q",0,"Water")</f>
+        <v>12858.051600018429</v>
       </c>
       <c r="D39">
-        <f t="shared" si="2"/>
-        <v>640.77321526474429</v>
+        <f>[1]!Props("D","T",B39,"Q",0,"Water")</f>
+        <v>640.7732152647435</v>
       </c>
       <c r="E39">
-        <f t="shared" si="3"/>
-        <v>77.050425987313758</v>
-      </c>
-      <c r="F39">
-        <f t="shared" si="4"/>
-        <v>1525.8683270564184</v>
-      </c>
-      <c r="G39">
-        <f t="shared" si="5"/>
-        <v>2666.031140557167</v>
+        <f>[1]!Props("D","T",B39,"Q",1,"Water")</f>
+        <v>77.05042598731238</v>
+      </c>
+      <c r="F39" t="e">
+        <f>[1]!Props("H","T",B39,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G39" t="e">
+        <f>[1]!Props("H","T",B39,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -2357,24 +2360,24 @@
         <v>613.15</v>
       </c>
       <c r="C40">
-        <f t="shared" si="1"/>
-        <v>14600.677371948052</v>
+        <f>[1]!Props("P","T",B40,"Q",0,"Water")</f>
+        <v>14600.677371948063</v>
       </c>
       <c r="D40">
-        <f t="shared" si="2"/>
-        <v>610.66759832473201</v>
+        <f>[1]!Props("D","T",B40,"Q",0,"Water")</f>
+        <v>610.66759832473281</v>
       </c>
       <c r="E40">
-        <f t="shared" si="3"/>
-        <v>92.758782507418118</v>
-      </c>
-      <c r="F40">
-        <f t="shared" si="4"/>
-        <v>1594.5289922369027</v>
-      </c>
-      <c r="G40">
-        <f t="shared" si="5"/>
-        <v>2621.8455755251762</v>
+        <f>[1]!Props("D","T",B40,"Q",1,"Water")</f>
+        <v>92.758782507416598</v>
+      </c>
+      <c r="F40" t="e">
+        <f>[1]!Props("H","T",B40,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G40" t="e">
+        <f>[1]!Props("H","T",B40,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -2386,24 +2389,24 @@
         <v>623.15</v>
       </c>
       <c r="C41">
-        <f t="shared" si="1"/>
-        <v>16529.415139004024</v>
+        <f>[1]!Props("P","T",B41,"Q",0,"Water")</f>
+        <v>16529.415139004064</v>
       </c>
       <c r="D41">
-        <f t="shared" si="2"/>
-        <v>574.70651653672405</v>
+        <f>[1]!Props("D","T",B41,"Q",0,"Water")</f>
+        <v>574.70651653672451</v>
       </c>
       <c r="E41">
-        <f t="shared" si="3"/>
-        <v>113.6056105016314</v>
-      </c>
-      <c r="F41">
-        <f t="shared" si="4"/>
-        <v>1670.8899067287159</v>
-      </c>
-      <c r="G41">
-        <f t="shared" si="5"/>
-        <v>2563.6367109445468</v>
+        <f>[1]!Props("D","T",B41,"Q",1,"Water")</f>
+        <v>113.60561050163348</v>
+      </c>
+      <c r="F41" t="e">
+        <f>[1]!Props("H","T",B41,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G41" t="e">
+        <f>[1]!Props("H","T",B41,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2415,24 +2418,24 @@
         <v>633.15</v>
       </c>
       <c r="C42">
-        <f t="shared" si="1"/>
-        <v>18666.006645644971</v>
+        <f>[1]!Props("P","T",B42,"Q",0,"Water")</f>
+        <v>18666.006645644644</v>
       </c>
       <c r="D42">
-        <f t="shared" si="2"/>
-        <v>527.59162939689577</v>
+        <f>[1]!Props("D","T",B42,"Q",0,"Water")</f>
+        <v>527.59162939688963</v>
       </c>
       <c r="E42">
-        <f t="shared" si="3"/>
-        <v>143.89841140943165</v>
-      </c>
-      <c r="F42">
-        <f t="shared" si="4"/>
-        <v>1761.6646205625905</v>
-      </c>
-      <c r="G42">
-        <f t="shared" si="5"/>
-        <v>2481.4924833322352</v>
+        <f>[1]!Props("D","T",B42,"Q",1,"Water")</f>
+        <v>143.89841140942264</v>
+      </c>
+      <c r="F42" t="e">
+        <f>[1]!Props("H","T",B42,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G42" t="e">
+        <f>[1]!Props("H","T",B42,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -2444,24 +2447,24 @@
         <v>643.15</v>
       </c>
       <c r="C43">
-        <f t="shared" si="1"/>
-        <v>21043.563147465771</v>
-      </c>
-      <c r="D43">
-        <f t="shared" si="2"/>
-        <v>451.42564747530241</v>
+        <f>[1]!Props("P","T",B43,"Q",0,"Water")</f>
+        <v>21043.56314746592</v>
+      </c>
+      <c r="D43" t="e">
+        <f>[1]!Props("D","T",B43,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="E43">
-        <f t="shared" si="3"/>
-        <v>201.83931641742618</v>
-      </c>
-      <c r="F43">
-        <f t="shared" si="4"/>
-        <v>1890.6872488661911</v>
-      </c>
-      <c r="G43">
-        <f t="shared" si="5"/>
-        <v>2334.5182916068688</v>
+        <f>[1]!Props("D","T",B43,"Q",1,"Water")</f>
+        <v>201.83931641744371</v>
+      </c>
+      <c r="F43" t="e">
+        <f>[1]!Props("H","T",B43,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G43" t="e">
+        <f>[1]!Props("H","T",B43,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -2470,28 +2473,28 @@
         <v>373.93600000000004</v>
       </c>
       <c r="B44" s="2">
-        <f t="shared" ref="B44" si="6">A44+273.15</f>
+        <f t="shared" ref="B44" si="1">A44+273.15</f>
         <v>647.08600000000001</v>
       </c>
       <c r="C44">
-        <f t="shared" ref="C44" si="7">[1]!Props("P","T",B44,"Q",0,"Water")</f>
-        <v>22061.3281318503</v>
+        <f>[1]!Props("P","T",B44,"Q",0,"Water")</f>
+        <v>22061.328131850038</v>
       </c>
       <c r="D44">
-        <f t="shared" ref="D44" si="8">[1]!Props("D","T",B44,"Q",0,"Water")</f>
-        <v>337.0441041609796</v>
+        <f>[1]!Props("D","T",B44,"Q",0,"Water")</f>
+        <v>337.04410411346163</v>
       </c>
       <c r="E44">
-        <f t="shared" ref="E44" si="9">[1]!Props("D","T",B44,"Q",1,"Water")</f>
-        <v>306.79658496624836</v>
-      </c>
-      <c r="F44">
-        <f t="shared" ref="F44" si="10">[1]!Props("H","T",B44,"Q",0,"Water")</f>
-        <v>2060.0042388190018</v>
-      </c>
-      <c r="G44">
-        <f t="shared" ref="G44" si="11">[1]!Props("H","T",B44,"Q",1,"Water")</f>
-        <v>2110.5585218700166</v>
+        <f>[1]!Props("D","T",B44,"Q",1,"Water")</f>
+        <v>306.79658492825473</v>
+      </c>
+      <c r="F44" t="e">
+        <f>[1]!Props("H","T",B44,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G44" t="e">
+        <f>[1]!Props("H","T",B44,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Perhaps the weirdest bug I have ever seen.  Calling ValidNumber(_h) and ValidNumber(_s) in CPState.cpp would not let the values go back through the DLL.  Changing them to boolean flags works fine now.  That has to be a bug in C++
</commit_message>
<xml_diff>
--- a/wrappers/Excel/TestExcel.xlsx
+++ b/wrappers/Excel/TestExcel.xlsx
@@ -235,121 +235,121 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>6.1220371526289217E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>42.021255884881164</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>83.914144952811796</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>125.73397341921785</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>167.5330355872081</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>209.34176132668705</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>251.18035191394253</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>293.06519282229988</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>335.01235325254447</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>377.03938647776687</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>419.16616289289658</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>461.4151895343303</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>503.81169242147121</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>546.38362438115269</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>589.16169048823679</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>632.17944178056644</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>675.47346558322408</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>719.08369096295746</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>763.05382639583047</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>807.43195145025493</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>852.27129446018387</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>897.63124444416621</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>943.5786700422118</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>990.18965507747453</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>1037.5518165790263</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>1085.7674588110503</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>1134.9579569891296</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>1185.2699943566126</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0</c:v>
+                  <c:v>1236.8846659592693</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0</c:v>
+                  <c:v>1290.0311497479681</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0</c:v>
+                  <c:v>1345.0079264161157</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0</c:v>
+                  <c:v>1402.2171260009688</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0</c:v>
+                  <c:v>1462.2236463970917</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0</c:v>
+                  <c:v>1525.8683270564179</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0</c:v>
+                  <c:v>1594.5289922369011</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0</c:v>
+                  <c:v>1670.8899067287161</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0</c:v>
+                  <c:v>1761.6646205625962</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0</c:v>
+                  <c:v>1890.6872488661784</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0</c:v>
+                  <c:v>2060.0042388923648</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -502,121 +502,121 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2500.9151916490418</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2519.2083189072159</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2537.4334043725835</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2555.545203294766</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2573.510322374003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2591.2888878672011</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2608.834872217727</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>2626.0964008315314</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>2643.0158813452254</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>2659.5300141957478</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>2675.5698844194635</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>2691.0613426859572</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>2705.9257657931835</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>2720.0811051450501</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>2733.4429731737555</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>2745.9254514300796</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>2757.4413489921203</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>2767.901762261462</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>2777.2149260216215</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>2785.2844447620487</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>2792.0070226267294</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>2797.2697683428019</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>2800.9470527725616</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>2802.8967584010438</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>2802.9556046252342</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>2800.9330729758321</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>2796.6032203853524</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>2789.6932193000084</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0</c:v>
+                  <c:v>2779.8667305294553</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0</c:v>
+                  <c:v>2766.6990506391335</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0</c:v>
+                  <c:v>2749.6387614002501</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0</c:v>
+                  <c:v>2727.9458789653868</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0</c:v>
+                  <c:v>2700.5857692409354</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0</c:v>
+                  <c:v>2666.0311405571751</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0</c:v>
+                  <c:v>2621.8455755251834</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0</c:v>
+                  <c:v>2563.6367109445368</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0</c:v>
+                  <c:v>2481.4924833322702</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0</c:v>
+                  <c:v>2334.5182916068165</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0</c:v>
+                  <c:v>2110.5585219387103</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -757,11 +757,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="119572736"/>
-        <c:axId val="119669120"/>
+        <c:axId val="128141568"/>
+        <c:axId val="128143744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="119572736"/>
+        <c:axId val="128141568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -790,12 +790,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119669120"/>
+        <c:crossAx val="128143744"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119669120"/>
+        <c:axId val="128143744"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -825,7 +825,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119572736"/>
+        <c:crossAx val="128141568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -847,15 +847,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1266,7 +1266,7 @@
       </c>
       <c r="B9">
         <f>[1]!Props("T","P",101.325,"Q",0,"REFPROP-Water")-273.15</f>
-        <v>99.974295847697647</v>
+        <v>-273.14999999999998</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>10</v>
@@ -1286,8 +1286,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,13 +1385,13 @@
         <f>[1]!Props("D","T",B6,"Q",1,"Water")</f>
         <v>4.8545757582901831E-3</v>
       </c>
-      <c r="F6" t="e">
+      <c r="F6">
         <f>[1]!Props("H","T",B6,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G6" t="e">
+        <v>6.1220371526289217E-4</v>
+      </c>
+      <c r="G6">
         <f>[1]!Props("H","T",B6,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2500.9151916490418</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1414,13 +1414,13 @@
         <f>[1]!Props("D","T",B7,"Q",1,"Water")</f>
         <v>9.4070520080230726E-3</v>
       </c>
-      <c r="F7" t="e">
+      <c r="F7">
         <f>[1]!Props("H","T",B7,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G7" t="e">
+        <v>42.021255884881164</v>
+      </c>
+      <c r="G7">
         <f>[1]!Props("H","T",B7,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2519.2083189072159</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1443,13 +1443,13 @@
         <f>[1]!Props("D","T",B8,"Q",1,"Water")</f>
         <v>1.7314008205457157E-2</v>
       </c>
-      <c r="F8" t="e">
+      <c r="F8">
         <f>[1]!Props("H","T",B8,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G8" t="e">
+        <v>83.914144952811796</v>
+      </c>
+      <c r="G8">
         <f>[1]!Props("H","T",B8,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2537.4334043725835</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1472,13 +1472,13 @@
         <f>[1]!Props("D","T",B9,"Q",1,"Water")</f>
         <v>3.0415211808982323E-2</v>
       </c>
-      <c r="F9" t="e">
+      <c r="F9">
         <f>[1]!Props("H","T",B9,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G9" t="e">
+        <v>125.73397341921785</v>
+      </c>
+      <c r="G9">
         <f>[1]!Props("H","T",B9,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2555.545203294766</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1501,13 +1501,13 @@
         <f>[1]!Props("D","T",B10,"Q",1,"Water")</f>
         <v>5.1242255801689097E-2</v>
       </c>
-      <c r="F10" t="e">
+      <c r="F10">
         <f>[1]!Props("H","T",B10,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G10" t="e">
+        <v>167.5330355872081</v>
+      </c>
+      <c r="G10">
         <f>[1]!Props("H","T",B10,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2573.510322374003</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1530,13 +1530,13 @@
         <f>[1]!Props("D","T",B11,"Q",1,"Water")</f>
         <v>8.3146842800445916E-2</v>
       </c>
-      <c r="F11" t="e">
+      <c r="F11">
         <f>[1]!Props("H","T",B11,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G11" t="e">
+        <v>209.34176132668705</v>
+      </c>
+      <c r="G11">
         <f>[1]!Props("H","T",B11,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2591.2888878672011</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1559,13 +1559,13 @@
         <f>[1]!Props("D","T",B12,"Q",1,"Water")</f>
         <v>0.13042522259659625</v>
       </c>
-      <c r="F12" t="e">
+      <c r="F12">
         <f>[1]!Props("H","T",B12,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G12" t="e">
+        <v>251.18035191394253</v>
+      </c>
+      <c r="G12">
         <f>[1]!Props("H","T",B12,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2608.834872217727</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1588,13 +1588,13 @@
         <f>[1]!Props("D","T",B13,"Q",1,"Water")</f>
         <v>0.19843073794182545</v>
       </c>
-      <c r="F13" t="e">
+      <c r="F13">
         <f>[1]!Props("H","T",B13,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G13" t="e">
+        <v>293.06519282229988</v>
+      </c>
+      <c r="G13">
         <f>[1]!Props("H","T",B13,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2626.0964008315314</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1617,13 +1617,13 @@
         <f>[1]!Props("D","T",B14,"Q",1,"Water")</f>
         <v>0.2936721347427359</v>
       </c>
-      <c r="F14" t="e">
+      <c r="F14">
         <f>[1]!Props("H","T",B14,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G14" t="e">
+        <v>335.01235325254447</v>
+      </c>
+      <c r="G14">
         <f>[1]!Props("H","T",B14,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2643.0158813452254</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1646,13 +1646,13 @@
         <f>[1]!Props("D","T",B15,"Q",1,"Water")</f>
         <v>0.42389794463171637</v>
       </c>
-      <c r="F15" t="e">
+      <c r="F15">
         <f>[1]!Props("H","T",B15,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G15" t="e">
+        <v>377.03938647776687</v>
+      </c>
+      <c r="G15">
         <f>[1]!Props("H","T",B15,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2659.5300141957478</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1675,13 +1675,13 @@
         <f>[1]!Props("D","T",B16,"Q",1,"Water")</f>
         <v>0.5981697919259753</v>
       </c>
-      <c r="F16" t="e">
+      <c r="F16">
         <f>[1]!Props("H","T",B16,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G16" t="e">
+        <v>419.16616289289658</v>
+      </c>
+      <c r="G16">
         <f>[1]!Props("H","T",B16,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2675.5698844194635</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1704,13 +1704,13 @@
         <f>[1]!Props("D","T",B17,"Q",1,"Water")</f>
         <v>0.82692959572358737</v>
       </c>
-      <c r="F17" t="e">
+      <c r="F17">
         <f>[1]!Props("H","T",B17,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G17" t="e">
+        <v>461.4151895343303</v>
+      </c>
+      <c r="G17">
         <f>[1]!Props("H","T",B17,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2691.0613426859572</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1733,13 +1733,13 @@
         <f>[1]!Props("D","T",B18,"Q",1,"Water")</f>
         <v>1.1220671917645244</v>
       </c>
-      <c r="F18" t="e">
+      <c r="F18">
         <f>[1]!Props("H","T",B18,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G18" t="e">
+        <v>503.81169242147121</v>
+      </c>
+      <c r="G18">
         <f>[1]!Props("H","T",B18,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2705.9257657931835</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1762,13 +1762,13 @@
         <f>[1]!Props("D","T",B19,"Q",1,"Water")</f>
         <v>1.4969959714828884</v>
       </c>
-      <c r="F19" t="e">
+      <c r="F19">
         <f>[1]!Props("H","T",B19,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G19" t="e">
+        <v>546.38362438115269</v>
+      </c>
+      <c r="G19">
         <f>[1]!Props("H","T",B19,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2720.0811051450501</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1791,13 +1791,13 @@
         <f>[1]!Props("D","T",B20,"Q",1,"Water")</f>
         <v>1.9667450045125305</v>
       </c>
-      <c r="F20" t="e">
+      <c r="F20">
         <f>[1]!Props("H","T",B20,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G20" t="e">
+        <v>589.16169048823679</v>
+      </c>
+      <c r="G20">
         <f>[1]!Props("H","T",B20,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2733.4429731737555</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1820,13 +1820,13 @@
         <f>[1]!Props("D","T",B21,"Q",1,"Water")</f>
         <v>2.5480771470961141</v>
       </c>
-      <c r="F21" t="e">
+      <c r="F21">
         <f>[1]!Props("H","T",B21,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G21" t="e">
+        <v>632.17944178056644</v>
+      </c>
+      <c r="G21">
         <f>[1]!Props("H","T",B21,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2745.9254514300796</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1849,13 +1849,13 @@
         <f>[1]!Props("D","T",B22,"Q",1,"Water")</f>
         <v>3.2596441977608386</v>
       </c>
-      <c r="F22" t="e">
+      <c r="F22">
         <f>[1]!Props("H","T",B22,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G22" t="e">
+        <v>675.47346558322408</v>
+      </c>
+      <c r="G22">
         <f>[1]!Props("H","T",B22,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2757.4413489921203</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1878,13 +1878,13 @@
         <f>[1]!Props("D","T",B23,"Q",1,"Water")</f>
         <v>4.1221925343361514</v>
       </c>
-      <c r="F23" t="e">
+      <c r="F23">
         <f>[1]!Props("H","T",B23,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G23" t="e">
+        <v>719.08369096295746</v>
+      </c>
+      <c r="G23">
         <f>[1]!Props("H","T",B23,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2767.901762261462</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1907,13 +1907,13 @@
         <f>[1]!Props("D","T",B24,"Q",1,"Water")</f>
         <v>5.1588361289185185</v>
       </c>
-      <c r="F24" t="e">
+      <c r="F24">
         <f>[1]!Props("H","T",B24,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G24" t="e">
+        <v>763.05382639583047</v>
+      </c>
+      <c r="G24">
         <f>[1]!Props("H","T",B24,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2777.2149260216215</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1936,13 +1936,13 @@
         <f>[1]!Props("D","T",B25,"Q",1,"Water")</f>
         <v>6.3954187812079395</v>
       </c>
-      <c r="F25" t="e">
+      <c r="F25">
         <f>[1]!Props("H","T",B25,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G25" t="e">
+        <v>807.43195145025493</v>
+      </c>
+      <c r="G25">
         <f>[1]!Props("H","T",B25,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2785.2844447620487</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1965,13 +1965,13 @@
         <f>[1]!Props("D","T",B26,"Q",1,"Water")</f>
         <v>7.860994516784042</v>
       </c>
-      <c r="F26" t="e">
+      <c r="F26">
         <f>[1]!Props("H","T",B26,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G26" t="e">
+        <v>852.27129446018387</v>
+      </c>
+      <c r="G26">
         <f>[1]!Props("H","T",B26,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2792.0070226267294</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1994,13 +1994,13 @@
         <f>[1]!Props("D","T",B27,"Q",1,"Water")</f>
         <v>9.5884655414267677</v>
       </c>
-      <c r="F27" t="e">
+      <c r="F27">
         <f>[1]!Props("H","T",B27,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G27" t="e">
+        <v>897.63124444416621</v>
+      </c>
+      <c r="G27">
         <f>[1]!Props("H","T",B27,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2797.2697683428019</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -2023,13 +2023,13 @@
         <f>[1]!Props("D","T",B28,"Q",1,"Water")</f>
         <v>11.615432874295058</v>
       </c>
-      <c r="F28" t="e">
+      <c r="F28">
         <f>[1]!Props("H","T",B28,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G28" t="e">
+        <v>943.5786700422118</v>
+      </c>
+      <c r="G28">
         <f>[1]!Props("H","T",B28,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2800.9470527725616</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -2052,13 +2052,13 @@
         <f>[1]!Props("D","T",B29,"Q",1,"Water")</f>
         <v>13.98533895750848</v>
       </c>
-      <c r="F29" t="e">
+      <c r="F29">
         <f>[1]!Props("H","T",B29,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G29" t="e">
+        <v>990.18965507747453</v>
+      </c>
+      <c r="G29">
         <f>[1]!Props("H","T",B29,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2802.8967584010438</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -2081,13 +2081,13 @@
         <f>[1]!Props("D","T",B30,"Q",1,"Water")</f>
         <v>16.749019301603251</v>
       </c>
-      <c r="F30" t="e">
+      <c r="F30">
         <f>[1]!Props("H","T",B30,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G30" t="e">
+        <v>1037.5518165790263</v>
+      </c>
+      <c r="G30">
         <f>[1]!Props("H","T",B30,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2802.9556046252342</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -2110,13 +2110,13 @@
         <f>[1]!Props("D","T",B31,"Q",1,"Water")</f>
         <v>19.966840438464651</v>
       </c>
-      <c r="F31" t="e">
+      <c r="F31">
         <f>[1]!Props("H","T",B31,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G31" t="e">
+        <v>1085.7674588110503</v>
+      </c>
+      <c r="G31">
         <f>[1]!Props("H","T",B31,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2800.9330729758321</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -2139,13 +2139,13 @@
         <f>[1]!Props("D","T",B32,"Q",1,"Water")</f>
         <v>23.711700367712265</v>
       </c>
-      <c r="F32" t="e">
+      <c r="F32">
         <f>[1]!Props("H","T",B32,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G32" t="e">
+        <v>1134.9579569891296</v>
+      </c>
+      <c r="G32">
         <f>[1]!Props("H","T",B32,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2796.6032203853524</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -2168,13 +2168,13 @@
         <f>[1]!Props("D","T",B33,"Q",1,"Water")</f>
         <v>28.07333562442464</v>
       </c>
-      <c r="F33" t="e">
+      <c r="F33">
         <f>[1]!Props("H","T",B33,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G33" t="e">
+        <v>1185.2699943566126</v>
+      </c>
+      <c r="G33">
         <f>[1]!Props("H","T",B33,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2789.6932193000084</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -2197,13 +2197,13 @@
         <f>[1]!Props("D","T",B34,"Q",1,"Water")</f>
         <v>33.164674054045683</v>
       </c>
-      <c r="F34" t="e">
+      <c r="F34">
         <f>[1]!Props("H","T",B34,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G34" t="e">
+        <v>1236.8846659592693</v>
+      </c>
+      <c r="G34">
         <f>[1]!Props("H","T",B34,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2779.8667305294553</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -2226,13 +2226,13 @@
         <f>[1]!Props("D","T",B35,"Q",1,"Water")</f>
         <v>39.131512960158695</v>
       </c>
-      <c r="F35" t="e">
+      <c r="F35">
         <f>[1]!Props("H","T",B35,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G35" t="e">
+        <v>1290.0311497479681</v>
+      </c>
+      <c r="G35">
         <f>[1]!Props("H","T",B35,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2766.6990506391335</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -2255,13 +2255,13 @@
         <f>[1]!Props("D","T",B36,"Q",1,"Water")</f>
         <v>46.167849523794111</v>
       </c>
-      <c r="F36" t="e">
+      <c r="F36">
         <f>[1]!Props("H","T",B36,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G36" t="e">
+        <v>1345.0079264161157</v>
+      </c>
+      <c r="G36">
         <f>[1]!Props("H","T",B36,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2749.6387614002501</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -2284,13 +2284,13 @@
         <f>[1]!Props("D","T",B37,"Q",1,"Water")</f>
         <v>54.541361541638153</v>
       </c>
-      <c r="F37" t="e">
+      <c r="F37">
         <f>[1]!Props("H","T",B37,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G37" t="e">
+        <v>1402.2171260009688</v>
+      </c>
+      <c r="G37">
         <f>[1]!Props("H","T",B37,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2727.9458789653868</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -2313,13 +2313,13 @@
         <f>[1]!Props("D","T",B38,"Q",1,"Water")</f>
         <v>64.638432419886186</v>
       </c>
-      <c r="F38" t="e">
+      <c r="F38">
         <f>[1]!Props("H","T",B38,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G38" t="e">
+        <v>1462.2236463970917</v>
+      </c>
+      <c r="G38">
         <f>[1]!Props("H","T",B38,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2700.5857692409354</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -2342,13 +2342,13 @@
         <f>[1]!Props("D","T",B39,"Q",1,"Water")</f>
         <v>77.05042598731238</v>
       </c>
-      <c r="F39" t="e">
+      <c r="F39">
         <f>[1]!Props("H","T",B39,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G39" t="e">
+        <v>1525.8683270564179</v>
+      </c>
+      <c r="G39">
         <f>[1]!Props("H","T",B39,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2666.0311405571751</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -2371,13 +2371,13 @@
         <f>[1]!Props("D","T",B40,"Q",1,"Water")</f>
         <v>92.758782507416598</v>
       </c>
-      <c r="F40" t="e">
+      <c r="F40">
         <f>[1]!Props("H","T",B40,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G40" t="e">
+        <v>1594.5289922369011</v>
+      </c>
+      <c r="G40">
         <f>[1]!Props("H","T",B40,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2621.8455755251834</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -2400,13 +2400,13 @@
         <f>[1]!Props("D","T",B41,"Q",1,"Water")</f>
         <v>113.60561050163348</v>
       </c>
-      <c r="F41" t="e">
+      <c r="F41">
         <f>[1]!Props("H","T",B41,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G41" t="e">
+        <v>1670.8899067287161</v>
+      </c>
+      <c r="G41">
         <f>[1]!Props("H","T",B41,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2563.6367109445368</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2429,13 +2429,13 @@
         <f>[1]!Props("D","T",B42,"Q",1,"Water")</f>
         <v>143.89841140942264</v>
       </c>
-      <c r="F42" t="e">
+      <c r="F42">
         <f>[1]!Props("H","T",B42,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G42" t="e">
+        <v>1761.6646205625962</v>
+      </c>
+      <c r="G42">
         <f>[1]!Props("H","T",B42,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2481.4924833322702</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -2450,21 +2450,21 @@
         <f>[1]!Props("P","T",B43,"Q",0,"Water")</f>
         <v>21043.56314746592</v>
       </c>
-      <c r="D43" t="e">
+      <c r="D43">
         <f>[1]!Props("D","T",B43,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
+        <v>451.42564747531384</v>
       </c>
       <c r="E43">
         <f>[1]!Props("D","T",B43,"Q",1,"Water")</f>
         <v>201.83931641744371</v>
       </c>
-      <c r="F43" t="e">
+      <c r="F43">
         <f>[1]!Props("H","T",B43,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G43" t="e">
+        <v>1890.6872488661784</v>
+      </c>
+      <c r="G43">
         <f>[1]!Props("H","T",B43,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2334.5182916068165</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -2488,13 +2488,13 @@
         <f>[1]!Props("D","T",B44,"Q",1,"Water")</f>
         <v>306.79658492825473</v>
       </c>
-      <c r="F44" t="e">
+      <c r="F44">
         <f>[1]!Props("H","T",B44,"Q",0,"Water")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G44" t="e">
+        <v>2060.0042388923648</v>
+      </c>
+      <c r="G44">
         <f>[1]!Props("H","T",B44,"Q",1,"Water")</f>
-        <v>#VALUE!</v>
+        <v>2110.5585219387103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Labview wrapper of CoolProp
</commit_message>
<xml_diff>
--- a/wrappers/Excel/TestExcel.xlsx
+++ b/wrappers/Excel/TestExcel.xlsx
@@ -757,11 +757,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="128141568"/>
-        <c:axId val="128143744"/>
+        <c:axId val="41765120"/>
+        <c:axId val="41767296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="128141568"/>
+        <c:axId val="41765120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -790,12 +790,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128143744"/>
+        <c:crossAx val="41767296"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="128143744"/>
+        <c:axId val="41767296"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -825,7 +825,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128141568"/>
+        <c:crossAx val="41765120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1266,7 +1266,7 @@
       </c>
       <c r="B9">
         <f>[1]!Props("T","P",101.325,"Q",0,"REFPROP-Water")-273.15</f>
-        <v>-273.14999999999998</v>
+        <v>99.974295847697647</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>10</v>
@@ -1287,7 +1287,7 @@
   <dimension ref="A2:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated CoolProp wrappers for Excel for 64-bit Excel
</commit_message>
<xml_diff>
--- a/wrappers/Excel/TestExcel.xlsx
+++ b/wrappers/Excel/TestExcel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sample calcs" sheetId="1" r:id="rId1"/>
@@ -757,11 +757,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="41765120"/>
-        <c:axId val="41767296"/>
+        <c:axId val="154097920"/>
+        <c:axId val="154100096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="41765120"/>
+        <c:axId val="154097920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -790,12 +790,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41767296"/>
+        <c:crossAx val="154100096"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="41767296"/>
+        <c:axId val="154100096"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -825,7 +825,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41765120"/>
+        <c:crossAx val="154097920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1188,8 +1188,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1286,7 +1286,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed Excel wrapper and improved examples
Signed-off-by: Ian Bell <ian.h.bell@gmail.com>
</commit_message>
<xml_diff>
--- a/wrappers/Excel/TestExcel.xlsx
+++ b/wrappers/Excel/TestExcel.xlsx
@@ -13,13 +13,14 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>Critical temperature of R410A:</t>
   </si>
@@ -54,9 +55,6 @@
   </si>
   <si>
     <t>Critical density of propane:</t>
-  </si>
-  <si>
-    <t>b) Enjoy!</t>
   </si>
   <si>
     <t>Saturation Table for water</t>
@@ -108,6 +106,24 @@
   <si>
     <t>(but calling REFPROP)</t>
   </si>
+  <si>
+    <t>b) Install the CoolProp Add-in</t>
+  </si>
+  <si>
+    <t>c) Enjoy!</t>
+  </si>
+  <si>
+    <t>Pa-s</t>
+  </si>
+  <si>
+    <t>CAS code of Water:</t>
+  </si>
+  <si>
+    <t>Example of an error:</t>
+  </si>
+  <si>
+    <t>Brine viscosity:</t>
+  </si>
 </sst>
 </file>
 
@@ -154,13 +170,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -206,7 +225,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -757,11 +775,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="154097920"/>
-        <c:axId val="154100096"/>
+        <c:axId val="137079040"/>
+        <c:axId val="137224576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="154097920"/>
+        <c:axId val="137079040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -783,19 +801,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154100096"/>
+        <c:crossAx val="137224576"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="154100096"/>
+        <c:axId val="137224576"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -818,14 +835,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154097920"/>
+        <c:crossAx val="137079040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -886,6 +902,7 @@
       <sheetName val="Sheet3"/>
     </sheetNames>
     <definedNames>
+      <definedName name="CAS_code"/>
       <definedName name="Props"/>
       <definedName name="Props1"/>
     </definedNames>
@@ -893,6 +910,29 @@
       <sheetData sheetId="0"/>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sample calcs"/>
+      <sheetName val="Water saturation table"/>
+      <sheetName val="Sheet3"/>
+      <sheetName val="CoolProp"/>
+    </sheetNames>
+    <definedNames>
+      <definedName name="Props"/>
+      <definedName name="Props1"/>
+    </definedNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1186,15 +1226,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1209,70 +1250,105 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B5">
+      <c r="B6" s="5">
         <f>[1]!Props1("R410A","Tcrit")</f>
         <v>344.49400000000003</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
+      <c r="B7" s="5">
         <f>[1]!Props1("Propane","rhocrit")</f>
         <v>220.47810000000001</v>
       </c>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <f>[1]!Props("D","T",298.15,"P",101.325,"Air")</f>
-        <v>1.1843184839089667</v>
-      </c>
       <c r="C7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <f>[1]!Props("T","P",101.325,"Q",0,"Water")-273.15</f>
-        <v>99.974295847683607</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
+      </c>
+      <c r="B8" s="5">
+        <f>[1]!Props("D","T",298.15,"P",101.325,"Air")</f>
+        <v>1.1843184838675069</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="5">
+        <f>[1]!Props("T","P",101.325,"Q",0,"Water")-273.15</f>
+        <v>99.974295847683209</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="5">
         <f>[1]!Props("T","P",101.325,"Q",0,"REFPROP-Water")-273.15</f>
         <v>99.974295847697647</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="5" t="str">
+        <f>[1]!CAS_code("Water")</f>
+        <v>7732-18-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="5" t="str">
+        <f>[1]!Props1("A","B")</f>
+        <v>CoolProp error: Fluid "A" is an invalid fluid</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="5">
+        <f>[1]!Props("V","T",300,"P",101.325,"EG-20%")</f>
+        <v>1.3814217810500947E-3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1298,7 +1374,7 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1307,50 +1383,50 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
@@ -1359,10 +1435,10 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1374,23 +1450,23 @@
         <v>273.16000009999999</v>
       </c>
       <c r="C6">
-        <f>[1]!Props("P","T",B6,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B6,"Q",0,"Water")</f>
         <v>0.61165477790576328</v>
       </c>
       <c r="D6">
-        <f>[1]!Props("D","T",B6,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B6,"Q",0,"Water")</f>
         <v>999.79252003842566</v>
       </c>
       <c r="E6">
-        <f>[1]!Props("D","T",B6,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B6,"Q",1,"Water")</f>
         <v>4.8545757582901831E-3</v>
       </c>
       <c r="F6">
-        <f>[1]!Props("H","T",B6,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B6,"Q",0,"Water")</f>
         <v>6.1220371526289217E-4</v>
       </c>
       <c r="G6">
-        <f>[1]!Props("H","T",B6,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B6,"Q",1,"Water")</f>
         <v>2500.9151916490418</v>
       </c>
     </row>
@@ -1403,23 +1479,23 @@
         <v>283.14999999999998</v>
       </c>
       <c r="C7">
-        <f>[1]!Props("P","T",B7,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B7,"Q",0,"Water")</f>
         <v>1.2281989260750077</v>
       </c>
       <c r="D7">
-        <f>[1]!Props("D","T",B7,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B7,"Q",0,"Water")</f>
         <v>999.65462464159361</v>
       </c>
       <c r="E7">
-        <f>[1]!Props("D","T",B7,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B7,"Q",1,"Water")</f>
         <v>9.4070520080230726E-3</v>
       </c>
       <c r="F7">
-        <f>[1]!Props("H","T",B7,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B7,"Q",0,"Water")</f>
         <v>42.021255884881164</v>
       </c>
       <c r="G7">
-        <f>[1]!Props("H","T",B7,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B7,"Q",1,"Water")</f>
         <v>2519.2083189072159</v>
       </c>
     </row>
@@ -1432,23 +1508,23 @@
         <v>293.14999999999998</v>
       </c>
       <c r="C8">
-        <f>[1]!Props("P","T",B8,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B8,"Q",0,"Water")</f>
         <v>2.3393181837875359</v>
       </c>
       <c r="D8">
-        <f>[1]!Props("D","T",B8,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B8,"Q",0,"Water")</f>
         <v>998.16180134317437</v>
       </c>
       <c r="E8">
-        <f>[1]!Props("D","T",B8,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B8,"Q",1,"Water")</f>
         <v>1.7314008205457157E-2</v>
       </c>
       <c r="F8">
-        <f>[1]!Props("H","T",B8,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B8,"Q",0,"Water")</f>
         <v>83.914144952811796</v>
       </c>
       <c r="G8">
-        <f>[1]!Props("H","T",B8,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B8,"Q",1,"Water")</f>
         <v>2537.4334043725835</v>
       </c>
     </row>
@@ -1461,23 +1537,23 @@
         <v>303.14999999999998</v>
       </c>
       <c r="C9">
-        <f>[1]!Props("P","T",B9,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B9,"Q",0,"Water")</f>
         <v>4.2469708407183706</v>
       </c>
       <c r="D9">
-        <f>[1]!Props("D","T",B9,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B9,"Q",0,"Water")</f>
         <v>995.60617747384663</v>
       </c>
       <c r="E9">
-        <f>[1]!Props("D","T",B9,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B9,"Q",1,"Water")</f>
         <v>3.0415211808982323E-2</v>
       </c>
       <c r="F9">
-        <f>[1]!Props("H","T",B9,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B9,"Q",0,"Water")</f>
         <v>125.73397341921785</v>
       </c>
       <c r="G9">
-        <f>[1]!Props("H","T",B9,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B9,"Q",1,"Water")</f>
         <v>2555.545203294766</v>
       </c>
     </row>
@@ -1490,23 +1566,23 @@
         <v>313.14999999999998</v>
       </c>
       <c r="C10">
-        <f>[1]!Props("P","T",B10,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B10,"Q",0,"Water")</f>
         <v>7.3849380739551265</v>
       </c>
       <c r="D10">
-        <f>[1]!Props("D","T",B10,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B10,"Q",0,"Water")</f>
         <v>992.17511534129721</v>
       </c>
       <c r="E10">
-        <f>[1]!Props("D","T",B10,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B10,"Q",1,"Water")</f>
         <v>5.1242255801689097E-2</v>
       </c>
       <c r="F10">
-        <f>[1]!Props("H","T",B10,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B10,"Q",0,"Water")</f>
         <v>167.5330355872081</v>
       </c>
       <c r="G10">
-        <f>[1]!Props("H","T",B10,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B10,"Q",1,"Water")</f>
         <v>2573.510322374003</v>
       </c>
     </row>
@@ -1519,23 +1595,23 @@
         <v>323.14999999999998</v>
       </c>
       <c r="C11">
-        <f>[1]!Props("P","T",B11,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B11,"Q",0,"Water")</f>
         <v>12.351945840547332</v>
       </c>
       <c r="D11">
-        <f>[1]!Props("D","T",B11,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B11,"Q",0,"Water")</f>
         <v>987.9962106111717</v>
       </c>
       <c r="E11">
-        <f>[1]!Props("D","T",B11,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B11,"Q",1,"Water")</f>
         <v>8.3146842800445916E-2</v>
       </c>
       <c r="F11">
-        <f>[1]!Props("H","T",B11,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B11,"Q",0,"Water")</f>
         <v>209.34176132668705</v>
       </c>
       <c r="G11">
-        <f>[1]!Props("H","T",B11,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B11,"Q",1,"Water")</f>
         <v>2591.2888878672011</v>
       </c>
     </row>
@@ -1548,23 +1624,23 @@
         <v>333.15</v>
       </c>
       <c r="C12">
-        <f>[1]!Props("P","T",B12,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B12,"Q",0,"Water")</f>
         <v>19.946434302277851</v>
       </c>
       <c r="D12">
-        <f>[1]!Props("D","T",B12,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B12,"Q",0,"Water")</f>
         <v>983.16021717833303</v>
       </c>
       <c r="E12">
-        <f>[1]!Props("D","T",B12,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B12,"Q",1,"Water")</f>
         <v>0.13042522259659625</v>
       </c>
       <c r="F12">
-        <f>[1]!Props("H","T",B12,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B12,"Q",0,"Water")</f>
         <v>251.18035191394253</v>
       </c>
       <c r="G12">
-        <f>[1]!Props("H","T",B12,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B12,"Q",1,"Water")</f>
         <v>2608.834872217727</v>
       </c>
     </row>
@@ -1577,23 +1653,23 @@
         <v>343.15</v>
       </c>
       <c r="C13">
-        <f>[1]!Props("P","T",B13,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B13,"Q",0,"Water")</f>
         <v>31.200930025942377</v>
       </c>
       <c r="D13">
-        <f>[1]!Props("D","T",B13,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B13,"Q",0,"Water")</f>
         <v>977.73365598192868</v>
       </c>
       <c r="E13">
-        <f>[1]!Props("D","T",B13,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B13,"Q",1,"Water")</f>
         <v>0.19843073794182545</v>
       </c>
       <c r="F13">
-        <f>[1]!Props("H","T",B13,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B13,"Q",0,"Water")</f>
         <v>293.06519282229988</v>
       </c>
       <c r="G13">
-        <f>[1]!Props("H","T",B13,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B13,"Q",1,"Water")</f>
         <v>2626.0964008315314</v>
       </c>
     </row>
@@ -1606,23 +1682,23 @@
         <v>353.15</v>
       </c>
       <c r="C14">
-        <f>[1]!Props("P","T",B14,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B14,"Q",0,"Water")</f>
         <v>47.414474030019207</v>
       </c>
       <c r="D14">
-        <f>[1]!Props("D","T",B14,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B14,"Q",0,"Water")</f>
         <v>971.76621871051145</v>
       </c>
       <c r="E14">
-        <f>[1]!Props("D","T",B14,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B14,"Q",1,"Water")</f>
         <v>0.2936721347427359</v>
       </c>
       <c r="F14">
-        <f>[1]!Props("H","T",B14,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B14,"Q",0,"Water")</f>
         <v>335.01235325254447</v>
       </c>
       <c r="G14">
-        <f>[1]!Props("H","T",B14,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B14,"Q",1,"Water")</f>
         <v>2643.0158813452254</v>
       </c>
     </row>
@@ -1635,23 +1711,23 @@
         <v>363.15</v>
       </c>
       <c r="C15">
-        <f>[1]!Props("P","T",B15,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B15,"Q",0,"Water")</f>
         <v>70.181765814537528</v>
       </c>
       <c r="D15">
-        <f>[1]!Props("D","T",B15,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B15,"Q",0,"Water")</f>
         <v>965.29532855043715</v>
       </c>
       <c r="E15">
-        <f>[1]!Props("D","T",B15,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B15,"Q",1,"Water")</f>
         <v>0.42389794463171637</v>
       </c>
       <c r="F15">
-        <f>[1]!Props("H","T",B15,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B15,"Q",0,"Water")</f>
         <v>377.03938647776687</v>
       </c>
       <c r="G15">
-        <f>[1]!Props("H","T",B15,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B15,"Q",1,"Water")</f>
         <v>2659.5300141957478</v>
       </c>
     </row>
@@ -1664,23 +1740,23 @@
         <v>373.15</v>
       </c>
       <c r="C16">
-        <f>[1]!Props("P","T",B16,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B16,"Q",0,"Water")</f>
         <v>101.41799666002106</v>
       </c>
       <c r="D16">
-        <f>[1]!Props("D","T",B16,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B16,"Q",0,"Water")</f>
         <v>958.34905160486005</v>
       </c>
       <c r="E16">
-        <f>[1]!Props("D","T",B16,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B16,"Q",1,"Water")</f>
         <v>0.5981697919259753</v>
       </c>
       <c r="F16">
-        <f>[1]!Props("H","T",B16,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B16,"Q",0,"Water")</f>
         <v>419.16616289289658</v>
       </c>
       <c r="G16">
-        <f>[1]!Props("H","T",B16,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B16,"Q",1,"Water")</f>
         <v>2675.5698844194635</v>
       </c>
     </row>
@@ -1693,23 +1769,23 @@
         <v>383.15</v>
       </c>
       <c r="C17">
-        <f>[1]!Props("P","T",B17,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B17,"Q",0,"Water")</f>
         <v>143.37871294940228</v>
       </c>
       <c r="D17">
-        <f>[1]!Props("D","T",B17,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B17,"Q",0,"Water")</f>
         <v>950.9480035889643</v>
       </c>
       <c r="E17">
-        <f>[1]!Props("D","T",B17,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B17,"Q",1,"Water")</f>
         <v>0.82692959572358737</v>
       </c>
       <c r="F17">
-        <f>[1]!Props("H","T",B17,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B17,"Q",0,"Water")</f>
         <v>461.4151895343303</v>
       </c>
       <c r="G17">
-        <f>[1]!Props("H","T",B17,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B17,"Q",1,"Water")</f>
         <v>2691.0613426859572</v>
       </c>
     </row>
@@ -1722,23 +1798,23 @@
         <v>393.15</v>
       </c>
       <c r="C18">
-        <f>[1]!Props("P","T",B18,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B18,"Q",0,"Water")</f>
         <v>198.67442047934145</v>
       </c>
       <c r="D18">
-        <f>[1]!Props("D","T",B18,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B18,"Q",0,"Water")</f>
         <v>943.106617430254</v>
       </c>
       <c r="E18">
-        <f>[1]!Props("D","T",B18,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B18,"Q",1,"Water")</f>
         <v>1.1220671917645244</v>
       </c>
       <c r="F18">
-        <f>[1]!Props("H","T",B18,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B18,"Q",0,"Water")</f>
         <v>503.81169242147121</v>
       </c>
       <c r="G18">
-        <f>[1]!Props("H","T",B18,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B18,"Q",1,"Water")</f>
         <v>2705.9257657931835</v>
       </c>
     </row>
@@ -1751,23 +1827,23 @@
         <v>403.15</v>
       </c>
       <c r="C19">
-        <f>[1]!Props("P","T",B19,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B19,"Q",0,"Water")</f>
         <v>270.27997678530858</v>
       </c>
       <c r="D19">
-        <f>[1]!Props("D","T",B19,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B19,"Q",0,"Water")</f>
         <v>934.83398660707985</v>
       </c>
       <c r="E19">
-        <f>[1]!Props("D","T",B19,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B19,"Q",1,"Water")</f>
         <v>1.4969959714828884</v>
       </c>
       <c r="F19">
-        <f>[1]!Props("H","T",B19,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B19,"Q",0,"Water")</f>
         <v>546.38362438115269</v>
       </c>
       <c r="G19">
-        <f>[1]!Props("H","T",B19,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B19,"Q",1,"Water")</f>
         <v>2720.0811051450501</v>
       </c>
     </row>
@@ -1780,23 +1856,23 @@
         <v>413.15</v>
       </c>
       <c r="C20">
-        <f>[1]!Props("P","T",B20,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B20,"Q",0,"Water")</f>
         <v>361.53909939988046</v>
       </c>
       <c r="D20">
-        <f>[1]!Props("D","T",B20,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B20,"Q",0,"Water")</f>
         <v>926.13441329112413</v>
       </c>
       <c r="E20">
-        <f>[1]!Props("D","T",B20,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B20,"Q",1,"Water")</f>
         <v>1.9667450045125305</v>
       </c>
       <c r="F20">
-        <f>[1]!Props("H","T",B20,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B20,"Q",0,"Water")</f>
         <v>589.16169048823679</v>
       </c>
       <c r="G20">
-        <f>[1]!Props("H","T",B20,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B20,"Q",1,"Water")</f>
         <v>2733.4429731737555</v>
       </c>
     </row>
@@ -1809,23 +1885,23 @@
         <v>423.15</v>
       </c>
       <c r="C21">
-        <f>[1]!Props("P","T",B21,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B21,"Q",0,"Water")</f>
         <v>476.16453797031113</v>
       </c>
       <c r="D21">
-        <f>[1]!Props("D","T",B21,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B21,"Q",0,"Water")</f>
         <v>917.00773926892555</v>
       </c>
       <c r="E21">
-        <f>[1]!Props("D","T",B21,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B21,"Q",1,"Water")</f>
         <v>2.5480771470961141</v>
       </c>
       <c r="F21">
-        <f>[1]!Props("H","T",B21,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B21,"Q",0,"Water")</f>
         <v>632.17944178056644</v>
       </c>
       <c r="G21">
-        <f>[1]!Props("H","T",B21,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B21,"Q",1,"Water")</f>
         <v>2745.9254514300796</v>
       </c>
     </row>
@@ -1838,23 +1914,23 @@
         <v>433.15</v>
       </c>
       <c r="C22">
-        <f>[1]!Props("P","T",B22,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B22,"Q",0,"Water")</f>
         <v>618.23462142577796</v>
       </c>
       <c r="D22">
-        <f>[1]!Props("D","T",B22,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B22,"Q",0,"Water")</f>
         <v>907.44950563407349</v>
       </c>
       <c r="E22">
-        <f>[1]!Props("D","T",B22,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B22,"Q",1,"Water")</f>
         <v>3.2596441977608386</v>
       </c>
       <c r="F22">
-        <f>[1]!Props("H","T",B22,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B22,"Q",0,"Water")</f>
         <v>675.47346558322408</v>
       </c>
       <c r="G22">
-        <f>[1]!Props("H","T",B22,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B22,"Q",1,"Water")</f>
         <v>2757.4413489921203</v>
       </c>
     </row>
@@ -1867,23 +1943,23 @@
         <v>443.15</v>
       </c>
       <c r="C23">
-        <f>[1]!Props("P","T",B23,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B23,"Q",0,"Water")</f>
         <v>792.18700698190401</v>
       </c>
       <c r="D23">
-        <f>[1]!Props("D","T",B23,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B23,"Q",0,"Water")</f>
         <v>897.45096587597288</v>
       </c>
       <c r="E23">
-        <f>[1]!Props("D","T",B23,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B23,"Q",1,"Water")</f>
         <v>4.1221925343361514</v>
       </c>
       <c r="F23">
-        <f>[1]!Props("H","T",B23,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B23,"Q",0,"Water")</f>
         <v>719.08369096295746</v>
       </c>
       <c r="G23">
-        <f>[1]!Props("H","T",B23,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B23,"Q",1,"Water")</f>
         <v>2767.901762261462</v>
       </c>
     </row>
@@ -1896,23 +1972,23 @@
         <v>453.15</v>
       </c>
       <c r="C24">
-        <f>[1]!Props("P","T",B24,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B24,"Q",0,"Water")</f>
         <v>1002.8105360782905</v>
       </c>
       <c r="D24">
-        <f>[1]!Props("D","T",B24,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B24,"Q",0,"Water")</f>
         <v>886.99896128082025</v>
       </c>
       <c r="E24">
-        <f>[1]!Props("D","T",B24,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B24,"Q",1,"Water")</f>
         <v>5.1588361289185185</v>
       </c>
       <c r="F24">
-        <f>[1]!Props("H","T",B24,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B24,"Q",0,"Water")</f>
         <v>763.05382639583047</v>
       </c>
       <c r="G24">
-        <f>[1]!Props("H","T",B24,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B24,"Q",1,"Water")</f>
         <v>2777.2149260216215</v>
       </c>
     </row>
@@ -1925,23 +2001,23 @@
         <v>463.15</v>
       </c>
       <c r="C25">
-        <f>[1]!Props("P","T",B25,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B25,"Q",0,"Water")</f>
         <v>1255.2361551605081</v>
       </c>
       <c r="D25">
-        <f>[1]!Props("D","T",B25,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B25,"Q",0,"Water")</f>
         <v>876.07565429885642</v>
       </c>
       <c r="E25">
-        <f>[1]!Props("D","T",B25,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B25,"Q",1,"Water")</f>
         <v>6.3954187812079395</v>
       </c>
       <c r="F25">
-        <f>[1]!Props("H","T",B25,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B25,"Q",0,"Water")</f>
         <v>807.43195145025493</v>
       </c>
       <c r="G25">
-        <f>[1]!Props("H","T",B25,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B25,"Q",1,"Water")</f>
         <v>2785.2844447620487</v>
       </c>
     </row>
@@ -1954,23 +2030,23 @@
         <v>473.15</v>
       </c>
       <c r="C26">
-        <f>[1]!Props("P","T",B26,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B26,"Q",0,"Water")</f>
         <v>1554.9279004667762</v>
       </c>
       <c r="D26">
-        <f>[1]!Props("D","T",B26,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B26,"Q",0,"Water")</f>
         <v>864.65810228712542</v>
       </c>
       <c r="E26">
-        <f>[1]!Props("D","T",B26,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B26,"Q",1,"Water")</f>
         <v>7.860994516784042</v>
       </c>
       <c r="F26">
-        <f>[1]!Props("H","T",B26,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B26,"Q",0,"Water")</f>
         <v>852.27129446018387</v>
       </c>
       <c r="G26">
-        <f>[1]!Props("H","T",B26,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B26,"Q",1,"Water")</f>
         <v>2792.0070226267294</v>
       </c>
     </row>
@@ -1983,23 +2059,23 @@
         <v>483.15</v>
       </c>
       <c r="C27">
-        <f>[1]!Props("P","T",B27,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B27,"Q",0,"Water")</f>
         <v>1907.6749935324397</v>
       </c>
       <c r="D27">
-        <f>[1]!Props("D","T",B27,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B27,"Q",0,"Water")</f>
         <v>852.71763851005721</v>
       </c>
       <c r="E27">
-        <f>[1]!Props("D","T",B27,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B27,"Q",1,"Water")</f>
         <v>9.5884655414267677</v>
       </c>
       <c r="F27">
-        <f>[1]!Props("H","T",B27,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B27,"Q",0,"Water")</f>
         <v>897.63124444416621</v>
       </c>
       <c r="G27">
-        <f>[1]!Props("H","T",B27,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B27,"Q",1,"Water")</f>
         <v>2797.2697683428019</v>
       </c>
     </row>
@@ -2012,23 +2088,23 @@
         <v>493.15</v>
       </c>
       <c r="C28">
-        <f>[1]!Props("P","T",B28,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B28,"Q",0,"Water")</f>
         <v>2319.5861701998538</v>
       </c>
       <c r="D28">
-        <f>[1]!Props("D","T",B28,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B28,"Q",0,"Water")</f>
         <v>840.21900675000336</v>
       </c>
       <c r="E28">
-        <f>[1]!Props("D","T",B28,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B28,"Q",1,"Water")</f>
         <v>11.615432874295058</v>
       </c>
       <c r="F28">
-        <f>[1]!Props("H","T",B28,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B28,"Q",0,"Water")</f>
         <v>943.5786700422118</v>
       </c>
       <c r="G28">
-        <f>[1]!Props("H","T",B28,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B28,"Q",1,"Water")</f>
         <v>2800.9470527725616</v>
       </c>
     </row>
@@ -2041,23 +2117,23 @@
         <v>503.15</v>
       </c>
       <c r="C29">
-        <f>[1]!Props("P","T",B29,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B29,"Q",0,"Water")</f>
         <v>2797.0874969297211</v>
       </c>
       <c r="D29">
-        <f>[1]!Props("D","T",B29,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B29,"Q",0,"Water")</f>
         <v>827.11916655179948</v>
       </c>
       <c r="E29">
-        <f>[1]!Props("D","T",B29,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B29,"Q",1,"Water")</f>
         <v>13.98533895750848</v>
       </c>
       <c r="F29">
-        <f>[1]!Props("H","T",B29,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B29,"Q",0,"Water")</f>
         <v>990.18965507747453</v>
       </c>
       <c r="G29">
-        <f>[1]!Props("H","T",B29,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B29,"Q",1,"Water")</f>
         <v>2802.8967584010438</v>
       </c>
     </row>
@@ -2070,23 +2146,23 @@
         <v>513.15</v>
       </c>
       <c r="C30">
-        <f>[1]!Props("P","T",B30,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B30,"Q",0,"Water")</f>
         <v>3346.9251442691252</v>
       </c>
       <c r="D30">
-        <f>[1]!Props("D","T",B30,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B30,"Q",0,"Water")</f>
         <v>813.36564216909892</v>
       </c>
       <c r="E30">
-        <f>[1]!Props("D","T",B30,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B30,"Q",1,"Water")</f>
         <v>16.749019301603251</v>
       </c>
       <c r="F30">
-        <f>[1]!Props("H","T",B30,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B30,"Q",0,"Water")</f>
         <v>1037.5518165790263</v>
       </c>
       <c r="G30">
-        <f>[1]!Props("H","T",B30,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B30,"Q",1,"Water")</f>
         <v>2802.9556046252342</v>
       </c>
     </row>
@@ -2099,23 +2175,23 @@
         <v>523.15</v>
       </c>
       <c r="C31">
-        <f>[1]!Props("P","T",B31,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B31,"Q",0,"Water")</f>
         <v>3976.1749306524707</v>
       </c>
       <c r="D31">
-        <f>[1]!Props("D","T",B31,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B31,"Q",0,"Water")</f>
         <v>798.89422022042186</v>
       </c>
       <c r="E31">
-        <f>[1]!Props("D","T",B31,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B31,"Q",1,"Water")</f>
         <v>19.966840438464651</v>
       </c>
       <c r="F31">
-        <f>[1]!Props("H","T",B31,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B31,"Q",0,"Water")</f>
         <v>1085.7674588110503</v>
       </c>
       <c r="G31">
-        <f>[1]!Props("H","T",B31,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B31,"Q",1,"Water")</f>
         <v>2800.9330729758321</v>
       </c>
     </row>
@@ -2128,23 +2204,23 @@
         <v>533.15</v>
       </c>
       <c r="C32">
-        <f>[1]!Props("P","T",B32,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B32,"Q",0,"Water")</f>
         <v>4692.260992299709</v>
       </c>
       <c r="D32">
-        <f>[1]!Props("D","T",B32,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B32,"Q",0,"Water")</f>
         <v>783.62569286973383</v>
       </c>
       <c r="E32">
-        <f>[1]!Props("D","T",B32,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B32,"Q",1,"Water")</f>
         <v>23.711700367712265</v>
       </c>
       <c r="F32">
-        <f>[1]!Props("H","T",B32,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B32,"Q",0,"Water")</f>
         <v>1134.9579569891296</v>
       </c>
       <c r="G32">
-        <f>[1]!Props("H","T",B32,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B32,"Q",1,"Water")</f>
         <v>2796.6032203853524</v>
       </c>
     </row>
@@ -2157,23 +2233,23 @@
         <v>543.15</v>
       </c>
       <c r="C33">
-        <f>[1]!Props("P","T",B33,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B33,"Q",0,"Water")</f>
         <v>5502.986783014605</v>
       </c>
       <c r="D33">
-        <f>[1]!Props("D","T",B33,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B33,"Q",0,"Water")</f>
         <v>767.46116679898125</v>
       </c>
       <c r="E33">
-        <f>[1]!Props("D","T",B33,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B33,"Q",1,"Water")</f>
         <v>28.07333562442464</v>
       </c>
       <c r="F33">
-        <f>[1]!Props("H","T",B33,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B33,"Q",0,"Water")</f>
         <v>1185.2699943566126</v>
       </c>
       <c r="G33">
-        <f>[1]!Props("H","T",B33,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B33,"Q",1,"Water")</f>
         <v>2789.6932193000084</v>
       </c>
     </row>
@@ -2186,23 +2262,23 @@
         <v>553.15</v>
       </c>
       <c r="C34">
-        <f>[1]!Props("P","T",B34,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B34,"Q",0,"Water")</f>
         <v>6416.582909532026</v>
       </c>
       <c r="D34">
-        <f>[1]!Props("D","T",B34,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B34,"Q",0,"Water")</f>
         <v>750.27516129988351</v>
       </c>
       <c r="E34">
-        <f>[1]!Props("D","T",B34,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B34,"Q",1,"Water")</f>
         <v>33.164674054045683</v>
       </c>
       <c r="F34">
-        <f>[1]!Props("H","T",B34,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B34,"Q",0,"Water")</f>
         <v>1236.8846659592693</v>
       </c>
       <c r="G34">
-        <f>[1]!Props("H","T",B34,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B34,"Q",1,"Water")</f>
         <v>2779.8667305294553</v>
       </c>
     </row>
@@ -2215,23 +2291,23 @@
         <v>563.15</v>
       </c>
       <c r="C35">
-        <f>[1]!Props("P","T",B35,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B35,"Q",0,"Water")</f>
         <v>7441.7783444212137</v>
       </c>
       <c r="D35">
-        <f>[1]!Props("D","T",B35,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B35,"Q",0,"Water")</f>
         <v>731.9051996436865</v>
       </c>
       <c r="E35">
-        <f>[1]!Props("D","T",B35,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B35,"Q",1,"Water")</f>
         <v>39.131512960158695</v>
       </c>
       <c r="F35">
-        <f>[1]!Props("H","T",B35,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B35,"Q",0,"Water")</f>
         <v>1290.0311497479681</v>
       </c>
       <c r="G35">
-        <f>[1]!Props("H","T",B35,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B35,"Q",1,"Water")</f>
         <v>2766.6990506391335</v>
       </c>
     </row>
@@ -2244,23 +2320,23 @@
         <v>573.15</v>
       </c>
       <c r="C36">
-        <f>[1]!Props("P","T",B36,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B36,"Q",0,"Water")</f>
         <v>8587.9049408353676</v>
       </c>
       <c r="D36">
-        <f>[1]!Props("D","T",B36,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B36,"Q",0,"Water")</f>
         <v>712.13563881961431</v>
       </c>
       <c r="E36">
-        <f>[1]!Props("D","T",B36,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B36,"Q",1,"Water")</f>
         <v>46.167849523794111</v>
       </c>
       <c r="F36">
-        <f>[1]!Props("H","T",B36,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B36,"Q",0,"Water")</f>
         <v>1345.0079264161157</v>
       </c>
       <c r="G36">
-        <f>[1]!Props("H","T",B36,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B36,"Q",1,"Water")</f>
         <v>2749.6387614002501</v>
       </c>
     </row>
@@ -2273,23 +2349,23 @@
         <v>583.15</v>
       </c>
       <c r="C37">
-        <f>[1]!Props("P","T",B37,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B37,"Q",0,"Water")</f>
         <v>9865.0512111820826</v>
       </c>
       <c r="D37">
-        <f>[1]!Props("D","T",B37,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B37,"Q",0,"Water")</f>
         <v>690.67154560984363</v>
       </c>
       <c r="E37">
-        <f>[1]!Props("D","T",B37,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B37,"Q",1,"Water")</f>
         <v>54.541361541638153</v>
       </c>
       <c r="F37">
-        <f>[1]!Props("H","T",B37,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B37,"Q",0,"Water")</f>
         <v>1402.2171260009688</v>
       </c>
       <c r="G37">
-        <f>[1]!Props("H","T",B37,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B37,"Q",1,"Water")</f>
         <v>2727.9458789653868</v>
       </c>
     </row>
@@ -2302,23 +2378,23 @@
         <v>593.15</v>
       </c>
       <c r="C38">
-        <f>[1]!Props("P","T",B38,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B38,"Q",0,"Water")</f>
         <v>11284.292927464725</v>
       </c>
       <c r="D38">
-        <f>[1]!Props("D","T",B38,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B38,"Q",0,"Water")</f>
         <v>667.09384803259525</v>
       </c>
       <c r="E38">
-        <f>[1]!Props("D","T",B38,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B38,"Q",1,"Water")</f>
         <v>64.638432419886186</v>
       </c>
       <c r="F38">
-        <f>[1]!Props("H","T",B38,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B38,"Q",0,"Water")</f>
         <v>1462.2236463970917</v>
       </c>
       <c r="G38">
-        <f>[1]!Props("H","T",B38,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B38,"Q",1,"Water")</f>
         <v>2700.5857692409354</v>
       </c>
     </row>
@@ -2331,23 +2407,23 @@
         <v>603.15</v>
       </c>
       <c r="C39">
-        <f>[1]!Props("P","T",B39,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B39,"Q",0,"Water")</f>
         <v>12858.051600018429</v>
       </c>
       <c r="D39">
-        <f>[1]!Props("D","T",B39,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B39,"Q",0,"Water")</f>
         <v>640.7732152647435</v>
       </c>
       <c r="E39">
-        <f>[1]!Props("D","T",B39,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B39,"Q",1,"Water")</f>
         <v>77.05042598731238</v>
       </c>
       <c r="F39">
-        <f>[1]!Props("H","T",B39,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B39,"Q",0,"Water")</f>
         <v>1525.8683270564179</v>
       </c>
       <c r="G39">
-        <f>[1]!Props("H","T",B39,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B39,"Q",1,"Water")</f>
         <v>2666.0311405571751</v>
       </c>
     </row>
@@ -2360,23 +2436,23 @@
         <v>613.15</v>
       </c>
       <c r="C40">
-        <f>[1]!Props("P","T",B40,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B40,"Q",0,"Water")</f>
         <v>14600.677371948063</v>
       </c>
       <c r="D40">
-        <f>[1]!Props("D","T",B40,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B40,"Q",0,"Water")</f>
         <v>610.66759832473281</v>
       </c>
       <c r="E40">
-        <f>[1]!Props("D","T",B40,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B40,"Q",1,"Water")</f>
         <v>92.758782507416598</v>
       </c>
       <c r="F40">
-        <f>[1]!Props("H","T",B40,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B40,"Q",0,"Water")</f>
         <v>1594.5289922369011</v>
       </c>
       <c r="G40">
-        <f>[1]!Props("H","T",B40,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B40,"Q",1,"Water")</f>
         <v>2621.8455755251834</v>
       </c>
     </row>
@@ -2389,23 +2465,23 @@
         <v>623.15</v>
       </c>
       <c r="C41">
-        <f>[1]!Props("P","T",B41,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B41,"Q",0,"Water")</f>
         <v>16529.415139004064</v>
       </c>
       <c r="D41">
-        <f>[1]!Props("D","T",B41,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B41,"Q",0,"Water")</f>
         <v>574.70651653672451</v>
       </c>
       <c r="E41">
-        <f>[1]!Props("D","T",B41,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B41,"Q",1,"Water")</f>
         <v>113.60561050163348</v>
       </c>
       <c r="F41">
-        <f>[1]!Props("H","T",B41,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B41,"Q",0,"Water")</f>
         <v>1670.8899067287161</v>
       </c>
       <c r="G41">
-        <f>[1]!Props("H","T",B41,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B41,"Q",1,"Water")</f>
         <v>2563.6367109445368</v>
       </c>
     </row>
@@ -2418,23 +2494,23 @@
         <v>633.15</v>
       </c>
       <c r="C42">
-        <f>[1]!Props("P","T",B42,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B42,"Q",0,"Water")</f>
         <v>18666.006645644644</v>
       </c>
       <c r="D42">
-        <f>[1]!Props("D","T",B42,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B42,"Q",0,"Water")</f>
         <v>527.59162939688963</v>
       </c>
       <c r="E42">
-        <f>[1]!Props("D","T",B42,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B42,"Q",1,"Water")</f>
         <v>143.89841140942264</v>
       </c>
       <c r="F42">
-        <f>[1]!Props("H","T",B42,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B42,"Q",0,"Water")</f>
         <v>1761.6646205625962</v>
       </c>
       <c r="G42">
-        <f>[1]!Props("H","T",B42,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B42,"Q",1,"Water")</f>
         <v>2481.4924833322702</v>
       </c>
     </row>
@@ -2447,29 +2523,29 @@
         <v>643.15</v>
       </c>
       <c r="C43">
-        <f>[1]!Props("P","T",B43,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B43,"Q",0,"Water")</f>
         <v>21043.56314746592</v>
       </c>
       <c r="D43">
-        <f>[1]!Props("D","T",B43,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B43,"Q",0,"Water")</f>
         <v>451.42564747531384</v>
       </c>
       <c r="E43">
-        <f>[1]!Props("D","T",B43,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B43,"Q",1,"Water")</f>
         <v>201.83931641744371</v>
       </c>
       <c r="F43">
-        <f>[1]!Props("H","T",B43,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B43,"Q",0,"Water")</f>
         <v>1890.6872488661784</v>
       </c>
       <c r="G43">
-        <f>[1]!Props("H","T",B43,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B43,"Q",1,"Water")</f>
         <v>2334.5182916068165</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f>[1]!Props1("Water","Tcrit")-0.01-273.15</f>
+        <f>[2]!Props1("Water","Tcrit")-0.01-273.15</f>
         <v>373.93600000000004</v>
       </c>
       <c r="B44" s="2">
@@ -2477,23 +2553,23 @@
         <v>647.08600000000001</v>
       </c>
       <c r="C44">
-        <f>[1]!Props("P","T",B44,"Q",0,"Water")</f>
+        <f>[2]!Props("P","T",B44,"Q",0,"Water")</f>
         <v>22061.328131850038</v>
       </c>
       <c r="D44">
-        <f>[1]!Props("D","T",B44,"Q",0,"Water")</f>
+        <f>[2]!Props("D","T",B44,"Q",0,"Water")</f>
         <v>337.04410411346163</v>
       </c>
       <c r="E44">
-        <f>[1]!Props("D","T",B44,"Q",1,"Water")</f>
+        <f>[2]!Props("D","T",B44,"Q",1,"Water")</f>
         <v>306.79658492825473</v>
       </c>
       <c r="F44">
-        <f>[1]!Props("H","T",B44,"Q",0,"Water")</f>
+        <f>[2]!Props("H","T",B44,"Q",0,"Water")</f>
         <v>2060.0042388923648</v>
       </c>
       <c r="G44">
-        <f>[1]!Props("H","T",B44,"Q",1,"Water")</f>
+        <f>[2]!Props("H","T",B44,"Q",1,"Water")</f>
         <v>2110.5585219387103</v>
       </c>
     </row>

</xml_diff>